<commit_message>
1st attempt  on ga, foundation has been covered
</commit_message>
<xml_diff>
--- a/csv/VisualPlotting.xlsx
+++ b/csv/VisualPlotting.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet3 (2)" sheetId="5" r:id="rId2"/>
     <sheet name="Sheet3 (3)" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet3 (4)" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="130">
   <si>
     <t>Room 1</t>
   </si>
@@ -390,12 +391,39 @@
   <si>
     <t>Mechtronics</t>
   </si>
+  <si>
+    <t>preferencePreferredNumberPeriodsDay</t>
+  </si>
+  <si>
+    <t>schedule_id </t>
+  </si>
+  <si>
+    <t>timetable_id</t>
+  </si>
+  <si>
+    <t>subject_class_id</t>
+  </si>
+  <si>
+    <t>schedule_slot</t>
+  </si>
+  <si>
+    <t>no.periods x no.days x no.rooms</t>
+  </si>
+  <si>
+    <t>total slots =</t>
+  </si>
+  <si>
+    <t>5 x 5 x 2</t>
+  </si>
+  <si>
+    <t>slots in total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,6 +446,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -658,7 +692,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -747,6 +781,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
@@ -756,8 +793,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1281,7 +1319,7 @@
       <c r="D5" s="12">
         <v>0</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="31" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -1316,7 +1354,7 @@
       <c r="D6" s="8">
         <v>1</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="32"/>
       <c r="F6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1349,7 +1387,7 @@
       <c r="D7" s="9">
         <v>2</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1383,7 +1421,7 @@
       <c r="D8" s="9">
         <v>3</v>
       </c>
-      <c r="E8" s="31"/>
+      <c r="E8" s="32"/>
       <c r="F8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1423,7 +1461,7 @@
       <c r="D9" s="7">
         <v>4</v>
       </c>
-      <c r="E9" s="31"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="5" t="s">
         <v>6</v>
       </c>
@@ -1463,7 +1501,7 @@
       <c r="D10" s="8">
         <v>5</v>
       </c>
-      <c r="E10" s="31"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1497,7 +1535,7 @@
       <c r="D11" s="9">
         <v>6</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1533,7 +1571,7 @@
       <c r="D12" s="9">
         <v>7</v>
       </c>
-      <c r="E12" s="31"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="3" t="s">
         <v>9</v>
       </c>
@@ -1564,7 +1602,7 @@
       <c r="D13" s="7">
         <v>8</v>
       </c>
-      <c r="E13" s="31"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="5" t="s">
         <v>10</v>
       </c>
@@ -1595,7 +1633,7 @@
       <c r="D14" s="8">
         <v>9</v>
       </c>
-      <c r="E14" s="31"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1626,7 +1664,7 @@
       <c r="D15" s="23">
         <v>10</v>
       </c>
-      <c r="E15" s="32"/>
+      <c r="E15" s="33"/>
       <c r="F15" s="22" t="s">
         <v>12</v>
       </c>
@@ -1657,7 +1695,7 @@
       <c r="D16" s="12">
         <v>11</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="31" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="11" t="s">
@@ -1692,7 +1730,7 @@
       <c r="D17" s="8">
         <v>12</v>
       </c>
-      <c r="E17" s="31"/>
+      <c r="E17" s="32"/>
       <c r="F17" s="4" t="s">
         <v>15</v>
       </c>
@@ -1725,7 +1763,7 @@
       <c r="D18" s="9">
         <v>13</v>
       </c>
-      <c r="E18" s="31"/>
+      <c r="E18" s="32"/>
       <c r="F18" s="3" t="s">
         <v>16</v>
       </c>
@@ -1756,7 +1794,7 @@
       <c r="D19" s="9">
         <v>14</v>
       </c>
-      <c r="E19" s="31"/>
+      <c r="E19" s="32"/>
       <c r="F19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1787,7 +1825,7 @@
       <c r="D20" s="7">
         <v>15</v>
       </c>
-      <c r="E20" s="31"/>
+      <c r="E20" s="32"/>
       <c r="F20" s="5" t="s">
         <v>18</v>
       </c>
@@ -1818,7 +1856,7 @@
       <c r="D21" s="8">
         <v>16</v>
       </c>
-      <c r="E21" s="31"/>
+      <c r="E21" s="32"/>
       <c r="F21" s="4" t="s">
         <v>19</v>
       </c>
@@ -1849,7 +1887,7 @@
       <c r="D22" s="9">
         <v>17</v>
       </c>
-      <c r="E22" s="31"/>
+      <c r="E22" s="32"/>
       <c r="F22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1880,7 +1918,7 @@
       <c r="D23" s="9">
         <v>18</v>
       </c>
-      <c r="E23" s="31"/>
+      <c r="E23" s="32"/>
       <c r="F23" s="3" t="s">
         <v>21</v>
       </c>
@@ -1911,7 +1949,7 @@
       <c r="D24" s="7">
         <v>19</v>
       </c>
-      <c r="E24" s="31"/>
+      <c r="E24" s="32"/>
       <c r="F24" s="5" t="s">
         <v>22</v>
       </c>
@@ -1942,7 +1980,7 @@
       <c r="D25" s="8">
         <v>20</v>
       </c>
-      <c r="E25" s="31"/>
+      <c r="E25" s="32"/>
       <c r="F25" s="4" t="s">
         <v>23</v>
       </c>
@@ -1973,7 +2011,7 @@
       <c r="D26" s="23">
         <v>21</v>
       </c>
-      <c r="E26" s="32"/>
+      <c r="E26" s="33"/>
       <c r="F26" s="22" t="s">
         <v>24</v>
       </c>
@@ -2004,7 +2042,7 @@
       <c r="D27" s="12">
         <v>22</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="31" t="s">
         <v>13</v>
       </c>
       <c r="F27" s="11" t="s">
@@ -2037,7 +2075,7 @@
       <c r="D28" s="8">
         <v>23</v>
       </c>
-      <c r="E28" s="31"/>
+      <c r="E28" s="32"/>
       <c r="F28" s="4" t="s">
         <v>15</v>
       </c>
@@ -2068,7 +2106,7 @@
       <c r="D29" s="9">
         <v>24</v>
       </c>
-      <c r="E29" s="31"/>
+      <c r="E29" s="32"/>
       <c r="F29" s="3" t="s">
         <v>16</v>
       </c>
@@ -2099,7 +2137,7 @@
       <c r="D30" s="9">
         <v>25</v>
       </c>
-      <c r="E30" s="31"/>
+      <c r="E30" s="32"/>
       <c r="F30" s="3" t="s">
         <v>17</v>
       </c>
@@ -2130,7 +2168,7 @@
       <c r="D31" s="7">
         <v>26</v>
       </c>
-      <c r="E31" s="31"/>
+      <c r="E31" s="32"/>
       <c r="F31" s="5" t="s">
         <v>18</v>
       </c>
@@ -2161,7 +2199,7 @@
       <c r="D32" s="8">
         <v>27</v>
       </c>
-      <c r="E32" s="31"/>
+      <c r="E32" s="32"/>
       <c r="F32" s="4" t="s">
         <v>19</v>
       </c>
@@ -2192,7 +2230,7 @@
       <c r="D33" s="9">
         <v>28</v>
       </c>
-      <c r="E33" s="31"/>
+      <c r="E33" s="32"/>
       <c r="F33" s="3" t="s">
         <v>20</v>
       </c>
@@ -2223,7 +2261,7 @@
       <c r="D34" s="9">
         <v>29</v>
       </c>
-      <c r="E34" s="31"/>
+      <c r="E34" s="32"/>
       <c r="F34" s="3" t="s">
         <v>21</v>
       </c>
@@ -2254,7 +2292,7 @@
       <c r="D35" s="7">
         <v>30</v>
       </c>
-      <c r="E35" s="31"/>
+      <c r="E35" s="32"/>
       <c r="F35" s="5" t="s">
         <v>22</v>
       </c>
@@ -2285,7 +2323,7 @@
       <c r="D36" s="8">
         <v>31</v>
       </c>
-      <c r="E36" s="31"/>
+      <c r="E36" s="32"/>
       <c r="F36" s="4" t="s">
         <v>23</v>
       </c>
@@ -2316,7 +2354,7 @@
       <c r="D37" s="23">
         <v>32</v>
       </c>
-      <c r="E37" s="32"/>
+      <c r="E37" s="33"/>
       <c r="F37" s="22" t="s">
         <v>24</v>
       </c>
@@ -2347,7 +2385,7 @@
       <c r="D38" s="12">
         <v>33</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="E38" s="31" t="s">
         <v>13</v>
       </c>
       <c r="F38" s="11" t="s">
@@ -2380,7 +2418,7 @@
       <c r="D39" s="8">
         <v>34</v>
       </c>
-      <c r="E39" s="31"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="4" t="s">
         <v>26</v>
       </c>
@@ -2411,7 +2449,7 @@
       <c r="D40" s="9">
         <v>35</v>
       </c>
-      <c r="E40" s="31"/>
+      <c r="E40" s="32"/>
       <c r="F40" s="3" t="s">
         <v>27</v>
       </c>
@@ -2442,7 +2480,7 @@
       <c r="D41" s="9">
         <v>36</v>
       </c>
-      <c r="E41" s="31"/>
+      <c r="E41" s="32"/>
       <c r="F41" s="3" t="s">
         <v>28</v>
       </c>
@@ -2473,7 +2511,7 @@
       <c r="D42" s="7">
         <v>37</v>
       </c>
-      <c r="E42" s="31"/>
+      <c r="E42" s="32"/>
       <c r="F42" s="5" t="s">
         <v>29</v>
       </c>
@@ -2504,7 +2542,7 @@
       <c r="D43" s="8">
         <v>38</v>
       </c>
-      <c r="E43" s="31"/>
+      <c r="E43" s="32"/>
       <c r="F43" s="4" t="s">
         <v>30</v>
       </c>
@@ -2535,7 +2573,7 @@
       <c r="D44" s="9">
         <v>39</v>
       </c>
-      <c r="E44" s="31"/>
+      <c r="E44" s="32"/>
       <c r="F44" s="3" t="s">
         <v>31</v>
       </c>
@@ -2566,7 +2604,7 @@
       <c r="D45" s="9">
         <v>40</v>
       </c>
-      <c r="E45" s="31"/>
+      <c r="E45" s="32"/>
       <c r="F45" s="3" t="s">
         <v>32</v>
       </c>
@@ -2597,7 +2635,7 @@
       <c r="D46" s="7">
         <v>41</v>
       </c>
-      <c r="E46" s="31"/>
+      <c r="E46" s="32"/>
       <c r="F46" s="5" t="s">
         <v>33</v>
       </c>
@@ -2628,7 +2666,7 @@
       <c r="D47" s="8">
         <v>42</v>
       </c>
-      <c r="E47" s="31"/>
+      <c r="E47" s="32"/>
       <c r="F47" s="4" t="s">
         <v>34</v>
       </c>
@@ -2659,7 +2697,7 @@
       <c r="D48" s="23">
         <v>43</v>
       </c>
-      <c r="E48" s="32"/>
+      <c r="E48" s="33"/>
       <c r="F48" s="22" t="s">
         <v>35</v>
       </c>
@@ -2690,7 +2728,7 @@
       <c r="D49" s="12">
         <v>44</v>
       </c>
-      <c r="E49" s="30" t="s">
+      <c r="E49" s="31" t="s">
         <v>13</v>
       </c>
       <c r="F49" s="11" t="s">
@@ -2723,7 +2761,7 @@
       <c r="D50" s="8">
         <v>45</v>
       </c>
-      <c r="E50" s="31"/>
+      <c r="E50" s="32"/>
       <c r="F50" s="4" t="s">
         <v>15</v>
       </c>
@@ -2754,7 +2792,7 @@
       <c r="D51" s="9">
         <v>46</v>
       </c>
-      <c r="E51" s="31"/>
+      <c r="E51" s="32"/>
       <c r="F51" s="3" t="s">
         <v>16</v>
       </c>
@@ -2785,7 +2823,7 @@
       <c r="D52" s="9">
         <v>47</v>
       </c>
-      <c r="E52" s="31"/>
+      <c r="E52" s="32"/>
       <c r="F52" s="3" t="s">
         <v>17</v>
       </c>
@@ -2816,7 +2854,7 @@
       <c r="D53" s="7">
         <v>48</v>
       </c>
-      <c r="E53" s="31"/>
+      <c r="E53" s="32"/>
       <c r="F53" s="5" t="s">
         <v>18</v>
       </c>
@@ -2847,7 +2885,7 @@
       <c r="D54" s="8">
         <v>49</v>
       </c>
-      <c r="E54" s="31"/>
+      <c r="E54" s="32"/>
       <c r="F54" s="4" t="s">
         <v>19</v>
       </c>
@@ -2878,7 +2916,7 @@
       <c r="D55" s="9">
         <v>50</v>
       </c>
-      <c r="E55" s="31"/>
+      <c r="E55" s="32"/>
       <c r="F55" s="3" t="s">
         <v>20</v>
       </c>
@@ -2909,7 +2947,7 @@
       <c r="D56" s="9">
         <v>51</v>
       </c>
-      <c r="E56" s="31"/>
+      <c r="E56" s="32"/>
       <c r="F56" s="3" t="s">
         <v>21</v>
       </c>
@@ -2940,7 +2978,7 @@
       <c r="D57" s="7">
         <v>52</v>
       </c>
-      <c r="E57" s="31"/>
+      <c r="E57" s="32"/>
       <c r="F57" s="5" t="s">
         <v>22</v>
       </c>
@@ -2971,7 +3009,7 @@
       <c r="D58" s="8">
         <v>53</v>
       </c>
-      <c r="E58" s="31"/>
+      <c r="E58" s="32"/>
       <c r="F58" s="4" t="s">
         <v>23</v>
       </c>
@@ -3002,7 +3040,7 @@
       <c r="D59" s="23">
         <v>54</v>
       </c>
-      <c r="E59" s="32"/>
+      <c r="E59" s="33"/>
       <c r="F59" s="22" t="s">
         <v>24</v>
       </c>
@@ -7272,7 +7310,7 @@
       <c r="D3" s="12">
         <v>0</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="31" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="11" t="s">
@@ -7335,7 +7373,7 @@
       <c r="D4" s="8">
         <v>1</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="4" t="s">
         <v>3</v>
       </c>
@@ -7394,7 +7432,7 @@
       <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="32"/>
       <c r="F5" s="3" t="s">
         <v>4</v>
       </c>
@@ -7455,7 +7493,7 @@
       <c r="D6" s="9">
         <v>3</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="32"/>
       <c r="F6" s="3" t="s">
         <v>5</v>
       </c>
@@ -7516,7 +7554,7 @@
       <c r="D7" s="9">
         <v>4</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
@@ -7575,7 +7613,7 @@
       <c r="D8" s="12">
         <v>5</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="31" t="s">
         <v>60</v>
       </c>
       <c r="F8" s="11" t="s">
@@ -7638,7 +7676,7 @@
       <c r="D9" s="8">
         <v>6</v>
       </c>
-      <c r="E9" s="31"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="4" t="s">
         <v>3</v>
       </c>
@@ -7699,7 +7737,7 @@
       <c r="D10" s="9">
         <v>7</v>
       </c>
-      <c r="E10" s="31"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="3" t="s">
         <v>4</v>
       </c>
@@ -7748,7 +7786,7 @@
       <c r="D11" s="9">
         <v>8</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="3" t="s">
         <v>5</v>
       </c>
@@ -7794,7 +7832,7 @@
       <c r="D12" s="9">
         <v>9</v>
       </c>
-      <c r="E12" s="31"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
@@ -9593,8 +9631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:P3"/>
+    <sheetView topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9703,7 +9741,7 @@
       <c r="S2" s="2">
         <v>201</v>
       </c>
-      <c r="T2" s="33">
+      <c r="T2" s="30">
         <v>101</v>
       </c>
       <c r="U2" s="2">
@@ -9735,7 +9773,7 @@
       <c r="D3" s="12">
         <v>0</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="31" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="11" t="s">
@@ -9773,7 +9811,7 @@
       <c r="S3" s="2">
         <v>201</v>
       </c>
-      <c r="T3" s="33">
+      <c r="T3" s="30">
         <v>102</v>
       </c>
       <c r="U3" s="2">
@@ -9805,7 +9843,7 @@
       <c r="D4" s="8">
         <v>1</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="4" t="s">
         <v>3</v>
       </c>
@@ -9841,7 +9879,7 @@
       <c r="S4" s="2">
         <v>201</v>
       </c>
-      <c r="T4" s="33">
+      <c r="T4" s="30">
         <v>103</v>
       </c>
       <c r="U4" s="2">
@@ -9873,7 +9911,7 @@
       <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="32"/>
       <c r="F5" s="3" t="s">
         <v>4</v>
       </c>
@@ -9909,7 +9947,7 @@
       <c r="S5" s="2">
         <v>202</v>
       </c>
-      <c r="T5" s="33">
+      <c r="T5" s="30">
         <v>104</v>
       </c>
       <c r="U5" s="2">
@@ -9941,7 +9979,7 @@
       <c r="D6" s="9">
         <v>3</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="32"/>
       <c r="F6" s="3" t="s">
         <v>5</v>
       </c>
@@ -9977,7 +10015,7 @@
       <c r="S6" s="2">
         <v>202</v>
       </c>
-      <c r="T6" s="33">
+      <c r="T6" s="30">
         <v>101</v>
       </c>
       <c r="U6" s="2">
@@ -10009,7 +10047,7 @@
       <c r="D7" s="9">
         <v>4</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
@@ -10043,7 +10081,7 @@
       <c r="S7" s="2">
         <v>202</v>
       </c>
-      <c r="T7" s="33">
+      <c r="T7" s="30">
         <v>102</v>
       </c>
       <c r="U7" s="2">
@@ -10075,7 +10113,7 @@
       <c r="D8" s="12">
         <v>5</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="31" t="s">
         <v>60</v>
       </c>
       <c r="F8" s="11" t="s">
@@ -10113,7 +10151,7 @@
       <c r="S8" s="2">
         <v>202</v>
       </c>
-      <c r="T8" s="33">
+      <c r="T8" s="30">
         <v>103</v>
       </c>
       <c r="U8" s="2">
@@ -10145,7 +10183,7 @@
       <c r="D9" s="8">
         <v>6</v>
       </c>
-      <c r="E9" s="31"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="4" t="s">
         <v>3</v>
       </c>
@@ -10181,7 +10219,7 @@
       <c r="S9" s="2">
         <v>202</v>
       </c>
-      <c r="T9" s="33">
+      <c r="T9" s="30">
         <v>104</v>
       </c>
       <c r="U9" s="2">
@@ -10213,7 +10251,7 @@
       <c r="D10" s="9">
         <v>7</v>
       </c>
-      <c r="E10" s="31"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="3" t="s">
         <v>4</v>
       </c>
@@ -10263,7 +10301,7 @@
       <c r="D11" s="9">
         <v>8</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="3" t="s">
         <v>5</v>
       </c>
@@ -10314,7 +10352,7 @@
       <c r="D12" s="9">
         <v>9</v>
       </c>
-      <c r="E12" s="31"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
@@ -12203,4 +12241,2724 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AA322"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="10" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="R2" sqref="R2:Z9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" customWidth="1"/>
+    <col min="11" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="27" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:27" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1">
+        <f>K38</f>
+        <v>401</v>
+      </c>
+      <c r="I1">
+        <v>402</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V1" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="W1" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="X1" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y1" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z1" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA1" s="27"/>
+    </row>
+    <row r="2" spans="2:27" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="str">
+        <f>L38</f>
+        <v>Room 1</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>101</v>
+      </c>
+      <c r="M2" s="2">
+        <v>201</v>
+      </c>
+      <c r="N2" s="2">
+        <v>301</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2">
+        <v>201</v>
+      </c>
+      <c r="T2" s="30">
+        <v>101</v>
+      </c>
+      <c r="U2" s="2">
+        <v>301</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W2" s="2">
+        <v>1</v>
+      </c>
+      <c r="X2" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="2"/>
+    </row>
+    <row r="3" spans="2:27" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="10">
+        <f>QUOTIENT(D3,5)+1</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="11">
+        <f>MOD(D3,5)+1</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="11">
+        <v>101</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <v>102</v>
+      </c>
+      <c r="M3" s="2">
+        <v>201</v>
+      </c>
+      <c r="N3" s="2">
+        <v>302</v>
+      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2">
+        <v>1</v>
+      </c>
+      <c r="S3" s="2">
+        <v>201</v>
+      </c>
+      <c r="T3" s="30">
+        <v>102</v>
+      </c>
+      <c r="U3" s="2">
+        <v>302</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W3" s="2">
+        <v>1</v>
+      </c>
+      <c r="X3" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA3" s="2"/>
+    </row>
+    <row r="4" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15">
+        <f t="shared" ref="B4:B12" si="0">QUOTIENT(D4,5)+1</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" ref="C4:C12" si="1">MOD(D4,5)+1</f>
+        <v>2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="4">
+        <v>102</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="K4" s="2">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2">
+        <v>103</v>
+      </c>
+      <c r="M4" s="2">
+        <v>201</v>
+      </c>
+      <c r="N4" s="2">
+        <v>303</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2">
+        <v>2</v>
+      </c>
+      <c r="S4" s="2">
+        <v>201</v>
+      </c>
+      <c r="T4" s="30">
+        <v>103</v>
+      </c>
+      <c r="U4" s="2">
+        <v>303</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W4" s="2">
+        <v>1</v>
+      </c>
+      <c r="X4" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA4" s="2"/>
+    </row>
+    <row r="5" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2</v>
+      </c>
+      <c r="E5" s="32"/>
+      <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="3">
+        <v>103</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" s="2">
+        <v>3</v>
+      </c>
+      <c r="L5" s="2">
+        <v>104</v>
+      </c>
+      <c r="M5" s="2">
+        <v>201</v>
+      </c>
+      <c r="N5" s="2">
+        <v>304</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2">
+        <v>3</v>
+      </c>
+      <c r="S5" s="2">
+        <v>202</v>
+      </c>
+      <c r="T5" s="30">
+        <v>104</v>
+      </c>
+      <c r="U5" s="2">
+        <v>304</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W5" s="2">
+        <v>1</v>
+      </c>
+      <c r="X5" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="2"/>
+    </row>
+    <row r="6" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D6" s="9">
+        <v>3</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="3">
+        <v>104</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="K6" s="2">
+        <v>4</v>
+      </c>
+      <c r="L6" s="2">
+        <v>101</v>
+      </c>
+      <c r="M6" s="2">
+        <v>202</v>
+      </c>
+      <c r="N6" s="2">
+        <v>301</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2">
+        <v>4</v>
+      </c>
+      <c r="S6" s="2">
+        <v>202</v>
+      </c>
+      <c r="T6" s="30">
+        <v>101</v>
+      </c>
+      <c r="U6" s="2">
+        <v>301</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W6" s="2">
+        <v>1</v>
+      </c>
+      <c r="X6" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA6" s="2"/>
+    </row>
+    <row r="7" spans="2:27" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D7" s="9">
+        <v>4</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="3">
+        <v>105</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="K7" s="2">
+        <v>5</v>
+      </c>
+      <c r="L7" s="2">
+        <v>102</v>
+      </c>
+      <c r="M7" s="2">
+        <v>202</v>
+      </c>
+      <c r="N7" s="2">
+        <v>302</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2">
+        <v>5</v>
+      </c>
+      <c r="S7" s="2">
+        <v>202</v>
+      </c>
+      <c r="T7" s="30">
+        <v>102</v>
+      </c>
+      <c r="U7" s="2">
+        <v>302</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W7" s="2">
+        <v>1</v>
+      </c>
+      <c r="X7" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA7" s="2"/>
+    </row>
+    <row r="8" spans="2:27" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C8" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D8" s="12">
+        <v>5</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="11">
+        <v>101</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="K8" s="2">
+        <v>6</v>
+      </c>
+      <c r="L8" s="2">
+        <v>103</v>
+      </c>
+      <c r="M8" s="2">
+        <v>202</v>
+      </c>
+      <c r="N8" s="2">
+        <v>303</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2">
+        <v>7</v>
+      </c>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2">
+        <v>6</v>
+      </c>
+      <c r="S8" s="2">
+        <v>202</v>
+      </c>
+      <c r="T8" s="30">
+        <v>103</v>
+      </c>
+      <c r="U8" s="2">
+        <v>303</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W8" s="2">
+        <v>1</v>
+      </c>
+      <c r="X8" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA8" s="2"/>
+    </row>
+    <row r="9" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D9" s="8">
+        <v>6</v>
+      </c>
+      <c r="E9" s="32"/>
+      <c r="F9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="4">
+        <v>102</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="K9" s="2">
+        <v>7</v>
+      </c>
+      <c r="L9" s="2">
+        <v>104</v>
+      </c>
+      <c r="M9" s="2">
+        <v>202</v>
+      </c>
+      <c r="N9" s="2">
+        <v>304</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2">
+        <v>8</v>
+      </c>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2">
+        <v>7</v>
+      </c>
+      <c r="S9" s="2">
+        <v>202</v>
+      </c>
+      <c r="T9" s="30">
+        <v>104</v>
+      </c>
+      <c r="U9" s="2">
+        <v>304</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W9" s="2">
+        <v>1</v>
+      </c>
+      <c r="X9" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA9" s="2"/>
+    </row>
+    <row r="10" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D10" s="9">
+        <v>7</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3">
+        <v>103</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="25"/>
+    </row>
+    <row r="11" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D11" s="9">
+        <v>8</v>
+      </c>
+      <c r="E11" s="32"/>
+      <c r="F11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="3">
+        <v>104</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+    </row>
+    <row r="12" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D12" s="9">
+        <v>9</v>
+      </c>
+      <c r="E12" s="32"/>
+      <c r="F12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="3">
+        <v>105</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+    </row>
+    <row r="13" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="29"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+    </row>
+    <row r="14" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="29"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+    </row>
+    <row r="15" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+    </row>
+    <row r="16" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="28"/>
+      <c r="C16" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+    </row>
+    <row r="17" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+    </row>
+    <row r="18" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="28"/>
+      <c r="C18" s="29">
+        <v>50</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+    </row>
+    <row r="19" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+    </row>
+    <row r="20" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+    </row>
+    <row r="21" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="K21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="S21" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="T21" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="U21" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="V21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+    </row>
+    <row r="22" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="K22" s="2">
+        <v>101</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N22" s="2">
+        <v>2</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2">
+        <v>0</v>
+      </c>
+      <c r="S22" s="2">
+        <v>1</v>
+      </c>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+    </row>
+    <row r="23" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="K23" s="2">
+        <v>102</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="N23" s="2">
+        <v>3</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2">
+        <v>1</v>
+      </c>
+      <c r="S23" s="2">
+        <v>1</v>
+      </c>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+    </row>
+    <row r="24" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="K24" s="2">
+        <v>103</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N24" s="2">
+        <v>3</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2">
+        <v>2</v>
+      </c>
+      <c r="S24" s="2">
+        <v>1</v>
+      </c>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+    </row>
+    <row r="25" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="K25" s="2">
+        <v>104</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="N25" s="2">
+        <v>2</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2">
+        <v>3</v>
+      </c>
+      <c r="S25" s="2">
+        <v>1</v>
+      </c>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+    </row>
+    <row r="26" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2">
+        <v>4</v>
+      </c>
+      <c r="S26" s="2">
+        <v>1</v>
+      </c>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
+    </row>
+    <row r="27" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="K27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2">
+        <v>5</v>
+      </c>
+      <c r="S27" s="2">
+        <v>1</v>
+      </c>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+    </row>
+    <row r="28" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="K28" s="2">
+        <v>201</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N28" s="2">
+        <v>1</v>
+      </c>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2">
+        <v>6</v>
+      </c>
+      <c r="S28" s="2">
+        <v>1</v>
+      </c>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+    </row>
+    <row r="29" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="K29" s="2">
+        <v>202</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N29" s="2">
+        <v>1</v>
+      </c>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2">
+        <v>7</v>
+      </c>
+      <c r="S29" s="2">
+        <v>1</v>
+      </c>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+    </row>
+    <row r="30" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2">
+        <v>8</v>
+      </c>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+    </row>
+    <row r="31" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="K31" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2">
+        <v>9</v>
+      </c>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+    </row>
+    <row r="32" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="K32" s="2">
+        <v>301</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2">
+        <v>10</v>
+      </c>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+    </row>
+    <row r="33" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="K33" s="2">
+        <v>302</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2">
+        <v>11</v>
+      </c>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+    </row>
+    <row r="34" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="K34" s="2">
+        <v>303</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2">
+        <v>12</v>
+      </c>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+    </row>
+    <row r="35" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="K35" s="2">
+        <v>304</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2">
+        <v>13</v>
+      </c>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+    </row>
+    <row r="36" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2">
+        <v>14</v>
+      </c>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+    </row>
+    <row r="37" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="K37" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2">
+        <v>15</v>
+      </c>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+    </row>
+    <row r="38" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="K38" s="2">
+        <v>401</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2">
+        <v>16</v>
+      </c>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+    </row>
+    <row r="39" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="K39" s="2">
+        <v>402</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2">
+        <v>17</v>
+      </c>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+    </row>
+    <row r="40" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2">
+        <v>18</v>
+      </c>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+    </row>
+    <row r="41" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="R41" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="R42" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="R43" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="R44" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="R45" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="R46" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="R47" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="R48" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="R49" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="R50" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="R51" s="2"/>
+    </row>
+    <row r="52" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="R52" s="2"/>
+    </row>
+    <row r="53" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="R53" s="2"/>
+    </row>
+    <row r="54" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="R54" s="2"/>
+    </row>
+    <row r="55" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="R55" s="2"/>
+    </row>
+    <row r="56" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="R56" s="2"/>
+    </row>
+    <row r="57" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="R57" s="2"/>
+    </row>
+    <row r="58" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="R58" s="2"/>
+    </row>
+    <row r="59" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="R59" s="2"/>
+    </row>
+    <row r="60" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="R60" s="2"/>
+    </row>
+    <row r="61" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="R61" s="2"/>
+    </row>
+    <row r="62" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="R62" s="2"/>
+    </row>
+    <row r="63" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="R63" s="2"/>
+    </row>
+    <row r="64" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="R64" s="2"/>
+    </row>
+    <row r="65" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="R65" s="2"/>
+    </row>
+    <row r="66" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="R66" s="2"/>
+    </row>
+    <row r="67" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="R67" s="2"/>
+    </row>
+    <row r="68" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="R68" s="2"/>
+    </row>
+    <row r="69" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="R69" s="2"/>
+    </row>
+    <row r="70" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="R70" s="2"/>
+    </row>
+    <row r="71" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="R71" s="2"/>
+    </row>
+    <row r="72" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="R72" s="2"/>
+    </row>
+    <row r="73" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="R73" s="2"/>
+    </row>
+    <row r="74" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="R74" s="2"/>
+    </row>
+    <row r="75" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="R75" s="2"/>
+    </row>
+    <row r="76" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="R76" s="2"/>
+    </row>
+    <row r="77" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="R77" s="2"/>
+    </row>
+    <row r="78" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="R78" s="2"/>
+    </row>
+    <row r="79" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
+      <c r="R79" s="2"/>
+    </row>
+    <row r="80" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="R80" s="2"/>
+    </row>
+    <row r="81" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="R81" s="2"/>
+    </row>
+    <row r="82" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="R82" s="2"/>
+    </row>
+    <row r="83" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="R83" s="2"/>
+    </row>
+    <row r="84" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+      <c r="R84" s="2"/>
+    </row>
+    <row r="85" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="R85" s="2"/>
+    </row>
+    <row r="86" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+      <c r="R86" s="2"/>
+    </row>
+    <row r="87" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="R87" s="2"/>
+    </row>
+    <row r="88" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
+      <c r="R88" s="2"/>
+    </row>
+    <row r="89" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+      <c r="R89" s="2"/>
+    </row>
+    <row r="90" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+      <c r="R90" s="2"/>
+    </row>
+    <row r="91" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+      <c r="R91" s="2"/>
+    </row>
+    <row r="92" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="R92" s="2"/>
+    </row>
+    <row r="93" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+      <c r="R93" s="2"/>
+    </row>
+    <row r="94" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
+      <c r="R94" s="2"/>
+    </row>
+    <row r="95" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+      <c r="R95" s="2"/>
+    </row>
+    <row r="96" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
+      <c r="R96" s="2"/>
+    </row>
+    <row r="97" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
+      <c r="R97" s="2"/>
+    </row>
+    <row r="98" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
+      <c r="R98" s="2"/>
+    </row>
+    <row r="99" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
+      <c r="R99" s="2"/>
+    </row>
+    <row r="100" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
+      <c r="R100" s="2"/>
+    </row>
+    <row r="101" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="R101" s="2"/>
+    </row>
+    <row r="102" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="R102" s="2"/>
+    </row>
+    <row r="103" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+      <c r="R103" s="2"/>
+    </row>
+    <row r="104" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+      <c r="R104" s="2"/>
+    </row>
+    <row r="105" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="R105" s="2"/>
+    </row>
+    <row r="106" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="R106" s="2"/>
+    </row>
+    <row r="107" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
+      <c r="R107" s="2"/>
+    </row>
+    <row r="108" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="R108" s="2"/>
+    </row>
+    <row r="109" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="R109" s="2"/>
+    </row>
+    <row r="110" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
+      <c r="R110" s="2"/>
+    </row>
+    <row r="111" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+      <c r="R111" s="2"/>
+    </row>
+    <row r="112" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="R112" s="2"/>
+    </row>
+    <row r="113" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+      <c r="R113" s="2"/>
+    </row>
+    <row r="114" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+    </row>
+    <row r="115" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+    </row>
+    <row r="116" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+    </row>
+    <row r="117" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
+    </row>
+    <row r="118" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
+    </row>
+    <row r="119" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H119" s="2"/>
+      <c r="I119" s="2"/>
+    </row>
+    <row r="120" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
+    </row>
+    <row r="121" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
+    </row>
+    <row r="122" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
+    </row>
+    <row r="123" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H123" s="2"/>
+      <c r="I123" s="2"/>
+    </row>
+    <row r="124" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
+    </row>
+    <row r="125" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H125" s="2"/>
+      <c r="I125" s="2"/>
+    </row>
+    <row r="126" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H126" s="2"/>
+      <c r="I126" s="2"/>
+    </row>
+    <row r="127" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H127" s="2"/>
+      <c r="I127" s="2"/>
+    </row>
+    <row r="128" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H128" s="2"/>
+      <c r="I128" s="2"/>
+    </row>
+    <row r="129" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H129" s="2"/>
+      <c r="I129" s="2"/>
+    </row>
+    <row r="130" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H130" s="2"/>
+      <c r="I130" s="2"/>
+    </row>
+    <row r="131" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H131" s="2"/>
+      <c r="I131" s="2"/>
+    </row>
+    <row r="132" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H132" s="2"/>
+      <c r="I132" s="2"/>
+    </row>
+    <row r="133" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H133" s="2"/>
+      <c r="I133" s="2"/>
+    </row>
+    <row r="134" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H134" s="2"/>
+      <c r="I134" s="2"/>
+    </row>
+    <row r="135" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H135" s="2"/>
+      <c r="I135" s="2"/>
+    </row>
+    <row r="136" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H136" s="2"/>
+      <c r="I136" s="2"/>
+    </row>
+    <row r="137" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H137" s="2"/>
+      <c r="I137" s="2"/>
+    </row>
+    <row r="138" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H138" s="2"/>
+      <c r="I138" s="2"/>
+    </row>
+    <row r="139" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H139" s="2"/>
+      <c r="I139" s="2"/>
+    </row>
+    <row r="140" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H140" s="2"/>
+      <c r="I140" s="2"/>
+    </row>
+    <row r="141" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H141" s="2"/>
+      <c r="I141" s="2"/>
+    </row>
+    <row r="142" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H142" s="2"/>
+      <c r="I142" s="2"/>
+    </row>
+    <row r="143" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H143" s="2"/>
+      <c r="I143" s="2"/>
+    </row>
+    <row r="144" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H144" s="2"/>
+      <c r="I144" s="2"/>
+    </row>
+    <row r="145" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H145" s="2"/>
+      <c r="I145" s="2"/>
+    </row>
+    <row r="146" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H146" s="2"/>
+      <c r="I146" s="2"/>
+    </row>
+    <row r="147" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H147" s="2"/>
+      <c r="I147" s="2"/>
+    </row>
+    <row r="148" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H148" s="2"/>
+      <c r="I148" s="2"/>
+    </row>
+    <row r="149" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H149" s="2"/>
+      <c r="I149" s="2"/>
+    </row>
+    <row r="150" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H150" s="2"/>
+      <c r="I150" s="2"/>
+    </row>
+    <row r="151" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H151" s="2"/>
+      <c r="I151" s="2"/>
+    </row>
+    <row r="152" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H152" s="2"/>
+      <c r="I152" s="2"/>
+    </row>
+    <row r="153" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H153" s="2"/>
+      <c r="I153" s="2"/>
+    </row>
+    <row r="154" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H154" s="2"/>
+      <c r="I154" s="2"/>
+    </row>
+    <row r="155" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H155" s="2"/>
+      <c r="I155" s="2"/>
+    </row>
+    <row r="156" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H156" s="2"/>
+      <c r="I156" s="2"/>
+    </row>
+    <row r="157" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H157" s="2"/>
+      <c r="I157" s="2"/>
+    </row>
+    <row r="158" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H158" s="2"/>
+      <c r="I158" s="2"/>
+    </row>
+    <row r="159" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H159" s="2"/>
+      <c r="I159" s="2"/>
+    </row>
+    <row r="160" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H160" s="2"/>
+      <c r="I160" s="2"/>
+    </row>
+    <row r="161" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H161" s="2"/>
+      <c r="I161" s="2"/>
+    </row>
+    <row r="162" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H162" s="2"/>
+      <c r="I162" s="2"/>
+    </row>
+    <row r="163" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H163" s="2"/>
+      <c r="I163" s="2"/>
+    </row>
+    <row r="164" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H164" s="2"/>
+      <c r="I164" s="2"/>
+    </row>
+    <row r="165" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H165" s="2"/>
+      <c r="I165" s="2"/>
+    </row>
+    <row r="166" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H166" s="2"/>
+      <c r="I166" s="2"/>
+    </row>
+    <row r="167" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H167" s="2"/>
+      <c r="I167" s="2"/>
+    </row>
+    <row r="168" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H168" s="2"/>
+      <c r="I168" s="2"/>
+    </row>
+    <row r="169" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H169" s="2"/>
+      <c r="I169" s="2"/>
+    </row>
+    <row r="170" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H170" s="2"/>
+      <c r="I170" s="2"/>
+    </row>
+    <row r="171" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H171" s="2"/>
+      <c r="I171" s="2"/>
+    </row>
+    <row r="172" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H172" s="2"/>
+      <c r="I172" s="2"/>
+    </row>
+    <row r="173" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H173" s="2"/>
+      <c r="I173" s="2"/>
+    </row>
+    <row r="174" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H174" s="2"/>
+      <c r="I174" s="2"/>
+    </row>
+    <row r="175" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H175" s="2"/>
+      <c r="I175" s="2"/>
+    </row>
+    <row r="176" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H176" s="2"/>
+      <c r="I176" s="2"/>
+    </row>
+    <row r="177" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H177" s="2"/>
+      <c r="I177" s="2"/>
+    </row>
+    <row r="178" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H178" s="2"/>
+      <c r="I178" s="2"/>
+    </row>
+    <row r="179" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H179" s="2"/>
+      <c r="I179" s="2"/>
+    </row>
+    <row r="180" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H180" s="2"/>
+      <c r="I180" s="2"/>
+    </row>
+    <row r="181" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H181" s="2"/>
+      <c r="I181" s="2"/>
+    </row>
+    <row r="182" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H182" s="2"/>
+      <c r="I182" s="2"/>
+    </row>
+    <row r="183" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H183" s="2"/>
+      <c r="I183" s="2"/>
+    </row>
+    <row r="184" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H184" s="2"/>
+      <c r="I184" s="2"/>
+    </row>
+    <row r="185" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H185" s="2"/>
+      <c r="I185" s="2"/>
+    </row>
+    <row r="186" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H186" s="2"/>
+      <c r="I186" s="2"/>
+    </row>
+    <row r="187" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H187" s="2"/>
+      <c r="I187" s="2"/>
+    </row>
+    <row r="188" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H188" s="2"/>
+      <c r="I188" s="2"/>
+    </row>
+    <row r="189" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H189" s="2"/>
+      <c r="I189" s="2"/>
+    </row>
+    <row r="190" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H190" s="2"/>
+      <c r="I190" s="2"/>
+    </row>
+    <row r="191" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H191" s="2"/>
+      <c r="I191" s="2"/>
+    </row>
+    <row r="192" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H192" s="2"/>
+      <c r="I192" s="2"/>
+    </row>
+    <row r="193" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H193" s="2"/>
+      <c r="I193" s="2"/>
+    </row>
+    <row r="194" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H194" s="2"/>
+      <c r="I194" s="2"/>
+    </row>
+    <row r="195" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H195" s="2"/>
+      <c r="I195" s="2"/>
+    </row>
+    <row r="196" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H196" s="2"/>
+      <c r="I196" s="2"/>
+    </row>
+    <row r="197" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H197" s="2"/>
+      <c r="I197" s="2"/>
+    </row>
+    <row r="198" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H198" s="2"/>
+      <c r="I198" s="2"/>
+    </row>
+    <row r="199" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H199" s="2"/>
+      <c r="I199" s="2"/>
+    </row>
+    <row r="200" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H200" s="2"/>
+      <c r="I200" s="2"/>
+    </row>
+    <row r="201" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H201" s="2"/>
+      <c r="I201" s="2"/>
+    </row>
+    <row r="202" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H202" s="2"/>
+      <c r="I202" s="2"/>
+    </row>
+    <row r="203" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H203" s="2"/>
+      <c r="I203" s="2"/>
+    </row>
+    <row r="204" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H204" s="2"/>
+      <c r="I204" s="2"/>
+    </row>
+    <row r="205" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H205" s="2"/>
+      <c r="I205" s="2"/>
+    </row>
+    <row r="206" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H206" s="2"/>
+      <c r="I206" s="2"/>
+    </row>
+    <row r="207" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H207" s="2"/>
+      <c r="I207" s="2"/>
+    </row>
+    <row r="208" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H208" s="2"/>
+      <c r="I208" s="2"/>
+    </row>
+    <row r="209" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H209" s="2"/>
+      <c r="I209" s="2"/>
+    </row>
+    <row r="210" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H210" s="2"/>
+      <c r="I210" s="2"/>
+    </row>
+    <row r="211" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H211" s="2"/>
+      <c r="I211" s="2"/>
+    </row>
+    <row r="212" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H212" s="2"/>
+      <c r="I212" s="2"/>
+    </row>
+    <row r="213" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H213" s="2"/>
+      <c r="I213" s="2"/>
+    </row>
+    <row r="214" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H214" s="2"/>
+      <c r="I214" s="2"/>
+    </row>
+    <row r="215" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H215" s="2"/>
+      <c r="I215" s="2"/>
+    </row>
+    <row r="216" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H216" s="2"/>
+      <c r="I216" s="2"/>
+    </row>
+    <row r="217" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H217" s="2"/>
+      <c r="I217" s="2"/>
+    </row>
+    <row r="218" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H218" s="2"/>
+      <c r="I218" s="2"/>
+    </row>
+    <row r="219" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H219" s="2"/>
+      <c r="I219" s="2"/>
+    </row>
+    <row r="220" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H220" s="2"/>
+      <c r="I220" s="2"/>
+    </row>
+    <row r="221" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H221" s="2"/>
+      <c r="I221" s="2"/>
+    </row>
+    <row r="222" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H222" s="2"/>
+      <c r="I222" s="2"/>
+    </row>
+    <row r="223" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H223" s="2"/>
+      <c r="I223" s="2"/>
+    </row>
+    <row r="224" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H224" s="2"/>
+      <c r="I224" s="2"/>
+    </row>
+    <row r="225" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H225" s="2"/>
+      <c r="I225" s="2"/>
+    </row>
+    <row r="226" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H226" s="2"/>
+      <c r="I226" s="2"/>
+    </row>
+    <row r="227" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H227" s="2"/>
+      <c r="I227" s="2"/>
+    </row>
+    <row r="228" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H228" s="2"/>
+      <c r="I228" s="2"/>
+    </row>
+    <row r="229" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H229" s="2"/>
+      <c r="I229" s="2"/>
+    </row>
+    <row r="230" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H230" s="2"/>
+      <c r="I230" s="2"/>
+    </row>
+    <row r="231" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H231" s="2"/>
+      <c r="I231" s="2"/>
+    </row>
+    <row r="232" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H232" s="2"/>
+      <c r="I232" s="2"/>
+    </row>
+    <row r="233" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H233" s="2"/>
+      <c r="I233" s="2"/>
+    </row>
+    <row r="234" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H234" s="2"/>
+      <c r="I234" s="2"/>
+    </row>
+    <row r="235" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H235" s="2"/>
+      <c r="I235" s="2"/>
+    </row>
+    <row r="236" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H236" s="2"/>
+      <c r="I236" s="2"/>
+    </row>
+    <row r="237" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H237" s="2"/>
+      <c r="I237" s="2"/>
+    </row>
+    <row r="238" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H238" s="2"/>
+      <c r="I238" s="2"/>
+    </row>
+    <row r="239" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H239" s="2"/>
+      <c r="I239" s="2"/>
+    </row>
+    <row r="240" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H240" s="2"/>
+      <c r="I240" s="2"/>
+    </row>
+    <row r="241" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H241" s="2"/>
+      <c r="I241" s="2"/>
+    </row>
+    <row r="242" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H242" s="2"/>
+      <c r="I242" s="2"/>
+    </row>
+    <row r="243" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H243" s="2"/>
+      <c r="I243" s="2"/>
+    </row>
+    <row r="244" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H244" s="2"/>
+      <c r="I244" s="2"/>
+    </row>
+    <row r="245" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H245" s="2"/>
+      <c r="I245" s="2"/>
+    </row>
+    <row r="246" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H246" s="2"/>
+      <c r="I246" s="2"/>
+    </row>
+    <row r="247" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H247" s="2"/>
+      <c r="I247" s="2"/>
+    </row>
+    <row r="248" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H248" s="2"/>
+      <c r="I248" s="2"/>
+    </row>
+    <row r="249" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H249" s="2"/>
+      <c r="I249" s="2"/>
+    </row>
+    <row r="250" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H250" s="2"/>
+      <c r="I250" s="2"/>
+    </row>
+    <row r="251" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H251" s="2"/>
+      <c r="I251" s="2"/>
+    </row>
+    <row r="252" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H252" s="2"/>
+      <c r="I252" s="2"/>
+    </row>
+    <row r="253" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H253" s="2"/>
+      <c r="I253" s="2"/>
+    </row>
+    <row r="254" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H254" s="2"/>
+      <c r="I254" s="2"/>
+    </row>
+    <row r="255" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H255" s="2"/>
+      <c r="I255" s="2"/>
+    </row>
+    <row r="256" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H256" s="2"/>
+      <c r="I256" s="2"/>
+    </row>
+    <row r="257" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H257" s="2"/>
+      <c r="I257" s="2"/>
+    </row>
+    <row r="258" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H258" s="2"/>
+      <c r="I258" s="2"/>
+    </row>
+    <row r="259" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H259" s="2"/>
+      <c r="I259" s="2"/>
+    </row>
+    <row r="260" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H260" s="2"/>
+      <c r="I260" s="2"/>
+    </row>
+    <row r="261" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H261" s="2"/>
+      <c r="I261" s="2"/>
+    </row>
+    <row r="262" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H262" s="2"/>
+      <c r="I262" s="2"/>
+    </row>
+    <row r="263" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H263" s="2"/>
+      <c r="I263" s="2"/>
+    </row>
+    <row r="264" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H264" s="2"/>
+      <c r="I264" s="2"/>
+    </row>
+    <row r="265" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H265" s="2"/>
+      <c r="I265" s="2"/>
+    </row>
+    <row r="266" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H266" s="2"/>
+      <c r="I266" s="2"/>
+    </row>
+    <row r="267" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H267" s="2"/>
+      <c r="I267" s="2"/>
+    </row>
+    <row r="268" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H268" s="2"/>
+      <c r="I268" s="2"/>
+    </row>
+    <row r="269" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H269" s="2"/>
+      <c r="I269" s="2"/>
+    </row>
+    <row r="270" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H270" s="2"/>
+      <c r="I270" s="2"/>
+    </row>
+    <row r="271" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H271" s="2"/>
+      <c r="I271" s="2"/>
+    </row>
+    <row r="272" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H272" s="2"/>
+      <c r="I272" s="2"/>
+    </row>
+    <row r="273" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H273" s="2"/>
+      <c r="I273" s="2"/>
+    </row>
+    <row r="274" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H274" s="2"/>
+      <c r="I274" s="2"/>
+    </row>
+    <row r="275" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H275" s="2"/>
+      <c r="I275" s="2"/>
+    </row>
+    <row r="276" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H276" s="2"/>
+      <c r="I276" s="2"/>
+    </row>
+    <row r="277" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H277" s="2"/>
+      <c r="I277" s="2"/>
+    </row>
+    <row r="278" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H278" s="2"/>
+      <c r="I278" s="2"/>
+    </row>
+    <row r="279" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H279" s="2"/>
+      <c r="I279" s="2"/>
+    </row>
+    <row r="280" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H280" s="2"/>
+      <c r="I280" s="2"/>
+    </row>
+    <row r="281" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H281" s="2"/>
+      <c r="I281" s="2"/>
+    </row>
+    <row r="282" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H282" s="2"/>
+      <c r="I282" s="2"/>
+    </row>
+    <row r="283" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H283" s="2"/>
+      <c r="I283" s="2"/>
+    </row>
+    <row r="284" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H284" s="2"/>
+      <c r="I284" s="2"/>
+    </row>
+    <row r="285" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H285" s="2"/>
+      <c r="I285" s="2"/>
+    </row>
+    <row r="286" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H286" s="2"/>
+      <c r="I286" s="2"/>
+    </row>
+    <row r="287" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H287" s="2"/>
+      <c r="I287" s="2"/>
+    </row>
+    <row r="288" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H288" s="2"/>
+      <c r="I288" s="2"/>
+    </row>
+    <row r="289" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H289" s="2"/>
+      <c r="I289" s="2"/>
+    </row>
+    <row r="290" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H290" s="2"/>
+      <c r="I290" s="2"/>
+    </row>
+    <row r="291" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H291" s="2"/>
+      <c r="I291" s="2"/>
+    </row>
+    <row r="292" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H292" s="2"/>
+      <c r="I292" s="2"/>
+    </row>
+    <row r="293" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H293" s="2"/>
+      <c r="I293" s="2"/>
+    </row>
+    <row r="294" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H294" s="2"/>
+      <c r="I294" s="2"/>
+    </row>
+    <row r="295" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H295" s="2"/>
+      <c r="I295" s="2"/>
+    </row>
+    <row r="296" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H296" s="2"/>
+      <c r="I296" s="2"/>
+    </row>
+    <row r="297" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H297" s="2"/>
+      <c r="I297" s="2"/>
+    </row>
+    <row r="298" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H298" s="2"/>
+      <c r="I298" s="2"/>
+    </row>
+    <row r="299" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H299" s="2"/>
+      <c r="I299" s="2"/>
+    </row>
+    <row r="300" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H300" s="2"/>
+      <c r="I300" s="2"/>
+    </row>
+    <row r="301" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H301" s="2"/>
+      <c r="I301" s="2"/>
+    </row>
+    <row r="302" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H302" s="2"/>
+      <c r="I302" s="2"/>
+    </row>
+    <row r="303" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H303" s="2"/>
+      <c r="I303" s="2"/>
+    </row>
+    <row r="304" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H304" s="2"/>
+      <c r="I304" s="2"/>
+    </row>
+    <row r="305" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H305" s="2"/>
+      <c r="I305" s="2"/>
+    </row>
+    <row r="306" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H306" s="2"/>
+      <c r="I306" s="2"/>
+    </row>
+    <row r="307" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H307" s="2"/>
+      <c r="I307" s="2"/>
+    </row>
+    <row r="308" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H308" s="2"/>
+      <c r="I308" s="2"/>
+    </row>
+    <row r="309" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H309" s="2"/>
+      <c r="I309" s="2"/>
+    </row>
+    <row r="310" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H310" s="2"/>
+      <c r="I310" s="2"/>
+    </row>
+    <row r="311" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H311" s="2"/>
+      <c r="I311" s="2"/>
+    </row>
+    <row r="312" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H312" s="2"/>
+      <c r="I312" s="2"/>
+    </row>
+    <row r="313" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H313" s="2"/>
+      <c r="I313" s="2"/>
+    </row>
+    <row r="314" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H314" s="2"/>
+      <c r="I314" s="2"/>
+    </row>
+    <row r="315" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H315" s="2"/>
+      <c r="I315" s="2"/>
+    </row>
+    <row r="316" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H316" s="2"/>
+      <c r="I316" s="2"/>
+    </row>
+    <row r="317" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H317" s="2"/>
+      <c r="I317" s="2"/>
+    </row>
+    <row r="318" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H318" s="2"/>
+      <c r="I318" s="2"/>
+    </row>
+    <row r="319" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H319" s="2"/>
+      <c r="I319" s="2"/>
+    </row>
+    <row r="320" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H320" s="2"/>
+      <c r="I320" s="2"/>
+    </row>
+    <row r="321" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H321" s="2"/>
+      <c r="I321" s="2"/>
+    </row>
+    <row r="322" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H322" s="2"/>
+      <c r="I322" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E3:E7"/>
+    <mergeCell ref="E8:E12"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="T2" location="'Sheet3 (3)'!K22" display="'Sheet3 (3)'!K22"/>
+    <hyperlink ref="T3" location="'Sheet3 (3)'!K23" display="'Sheet3 (3)'!K23"/>
+    <hyperlink ref="T4" location="'Sheet3 (3)'!K24" display="'Sheet3 (3)'!K24"/>
+    <hyperlink ref="T5" location="'Sheet3 (3)'!K25" display="'Sheet3 (3)'!K25"/>
+    <hyperlink ref="T6" location="'Sheet3 (3)'!K22" display="'Sheet3 (3)'!K22"/>
+    <hyperlink ref="T7" location="'Sheet3 (3)'!K23" display="'Sheet3 (3)'!K23"/>
+    <hyperlink ref="T8" location="'Sheet3 (3)'!K24" display="'Sheet3 (3)'!K24"/>
+    <hyperlink ref="T9" location="'Sheet3 (3)'!K25" display="'Sheet3 (3)'!K25"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
correct misplaced parameters in preferences and subjectclasses
</commit_message>
<xml_diff>
--- a/csv/VisualPlotting.xlsx
+++ b/csv/VisualPlotting.xlsx
@@ -784,6 +784,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
@@ -792,10 +796,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1319,7 +1319,7 @@
       <c r="D5" s="12">
         <v>0</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -1354,7 +1354,7 @@
       <c r="D6" s="8">
         <v>1</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1387,7 +1387,7 @@
       <c r="D7" s="9">
         <v>2</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1421,7 +1421,7 @@
       <c r="D8" s="9">
         <v>3</v>
       </c>
-      <c r="E8" s="32"/>
+      <c r="E8" s="34"/>
       <c r="F8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1461,7 +1461,7 @@
       <c r="D9" s="7">
         <v>4</v>
       </c>
-      <c r="E9" s="32"/>
+      <c r="E9" s="34"/>
       <c r="F9" s="5" t="s">
         <v>6</v>
       </c>
@@ -1501,7 +1501,7 @@
       <c r="D10" s="8">
         <v>5</v>
       </c>
-      <c r="E10" s="32"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1535,7 +1535,7 @@
       <c r="D11" s="9">
         <v>6</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="34"/>
       <c r="F11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1571,7 +1571,7 @@
       <c r="D12" s="9">
         <v>7</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="34"/>
       <c r="F12" s="3" t="s">
         <v>9</v>
       </c>
@@ -1602,7 +1602,7 @@
       <c r="D13" s="7">
         <v>8</v>
       </c>
-      <c r="E13" s="32"/>
+      <c r="E13" s="34"/>
       <c r="F13" s="5" t="s">
         <v>10</v>
       </c>
@@ -1633,7 +1633,7 @@
       <c r="D14" s="8">
         <v>9</v>
       </c>
-      <c r="E14" s="32"/>
+      <c r="E14" s="34"/>
       <c r="F14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1664,7 +1664,7 @@
       <c r="D15" s="23">
         <v>10</v>
       </c>
-      <c r="E15" s="33"/>
+      <c r="E15" s="35"/>
       <c r="F15" s="22" t="s">
         <v>12</v>
       </c>
@@ -1695,7 +1695,7 @@
       <c r="D16" s="12">
         <v>11</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="11" t="s">
@@ -1730,7 +1730,7 @@
       <c r="D17" s="8">
         <v>12</v>
       </c>
-      <c r="E17" s="32"/>
+      <c r="E17" s="34"/>
       <c r="F17" s="4" t="s">
         <v>15</v>
       </c>
@@ -1763,7 +1763,7 @@
       <c r="D18" s="9">
         <v>13</v>
       </c>
-      <c r="E18" s="32"/>
+      <c r="E18" s="34"/>
       <c r="F18" s="3" t="s">
         <v>16</v>
       </c>
@@ -1794,7 +1794,7 @@
       <c r="D19" s="9">
         <v>14</v>
       </c>
-      <c r="E19" s="32"/>
+      <c r="E19" s="34"/>
       <c r="F19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1825,7 +1825,7 @@
       <c r="D20" s="7">
         <v>15</v>
       </c>
-      <c r="E20" s="32"/>
+      <c r="E20" s="34"/>
       <c r="F20" s="5" t="s">
         <v>18</v>
       </c>
@@ -1856,7 +1856,7 @@
       <c r="D21" s="8">
         <v>16</v>
       </c>
-      <c r="E21" s="32"/>
+      <c r="E21" s="34"/>
       <c r="F21" s="4" t="s">
         <v>19</v>
       </c>
@@ -1887,7 +1887,7 @@
       <c r="D22" s="9">
         <v>17</v>
       </c>
-      <c r="E22" s="32"/>
+      <c r="E22" s="34"/>
       <c r="F22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1918,7 +1918,7 @@
       <c r="D23" s="9">
         <v>18</v>
       </c>
-      <c r="E23" s="32"/>
+      <c r="E23" s="34"/>
       <c r="F23" s="3" t="s">
         <v>21</v>
       </c>
@@ -1949,7 +1949,7 @@
       <c r="D24" s="7">
         <v>19</v>
       </c>
-      <c r="E24" s="32"/>
+      <c r="E24" s="34"/>
       <c r="F24" s="5" t="s">
         <v>22</v>
       </c>
@@ -1980,7 +1980,7 @@
       <c r="D25" s="8">
         <v>20</v>
       </c>
-      <c r="E25" s="32"/>
+      <c r="E25" s="34"/>
       <c r="F25" s="4" t="s">
         <v>23</v>
       </c>
@@ -2011,7 +2011,7 @@
       <c r="D26" s="23">
         <v>21</v>
       </c>
-      <c r="E26" s="33"/>
+      <c r="E26" s="35"/>
       <c r="F26" s="22" t="s">
         <v>24</v>
       </c>
@@ -2042,7 +2042,7 @@
       <c r="D27" s="12">
         <v>22</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F27" s="11" t="s">
@@ -2075,7 +2075,7 @@
       <c r="D28" s="8">
         <v>23</v>
       </c>
-      <c r="E28" s="32"/>
+      <c r="E28" s="34"/>
       <c r="F28" s="4" t="s">
         <v>15</v>
       </c>
@@ -2106,7 +2106,7 @@
       <c r="D29" s="9">
         <v>24</v>
       </c>
-      <c r="E29" s="32"/>
+      <c r="E29" s="34"/>
       <c r="F29" s="3" t="s">
         <v>16</v>
       </c>
@@ -2137,7 +2137,7 @@
       <c r="D30" s="9">
         <v>25</v>
       </c>
-      <c r="E30" s="32"/>
+      <c r="E30" s="34"/>
       <c r="F30" s="3" t="s">
         <v>17</v>
       </c>
@@ -2168,7 +2168,7 @@
       <c r="D31" s="7">
         <v>26</v>
       </c>
-      <c r="E31" s="32"/>
+      <c r="E31" s="34"/>
       <c r="F31" s="5" t="s">
         <v>18</v>
       </c>
@@ -2199,7 +2199,7 @@
       <c r="D32" s="8">
         <v>27</v>
       </c>
-      <c r="E32" s="32"/>
+      <c r="E32" s="34"/>
       <c r="F32" s="4" t="s">
         <v>19</v>
       </c>
@@ -2230,7 +2230,7 @@
       <c r="D33" s="9">
         <v>28</v>
       </c>
-      <c r="E33" s="32"/>
+      <c r="E33" s="34"/>
       <c r="F33" s="3" t="s">
         <v>20</v>
       </c>
@@ -2261,7 +2261,7 @@
       <c r="D34" s="9">
         <v>29</v>
       </c>
-      <c r="E34" s="32"/>
+      <c r="E34" s="34"/>
       <c r="F34" s="3" t="s">
         <v>21</v>
       </c>
@@ -2292,7 +2292,7 @@
       <c r="D35" s="7">
         <v>30</v>
       </c>
-      <c r="E35" s="32"/>
+      <c r="E35" s="34"/>
       <c r="F35" s="5" t="s">
         <v>22</v>
       </c>
@@ -2323,7 +2323,7 @@
       <c r="D36" s="8">
         <v>31</v>
       </c>
-      <c r="E36" s="32"/>
+      <c r="E36" s="34"/>
       <c r="F36" s="4" t="s">
         <v>23</v>
       </c>
@@ -2354,7 +2354,7 @@
       <c r="D37" s="23">
         <v>32</v>
       </c>
-      <c r="E37" s="33"/>
+      <c r="E37" s="35"/>
       <c r="F37" s="22" t="s">
         <v>24</v>
       </c>
@@ -2385,7 +2385,7 @@
       <c r="D38" s="12">
         <v>33</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F38" s="11" t="s">
@@ -2418,7 +2418,7 @@
       <c r="D39" s="8">
         <v>34</v>
       </c>
-      <c r="E39" s="32"/>
+      <c r="E39" s="34"/>
       <c r="F39" s="4" t="s">
         <v>26</v>
       </c>
@@ -2449,7 +2449,7 @@
       <c r="D40" s="9">
         <v>35</v>
       </c>
-      <c r="E40" s="32"/>
+      <c r="E40" s="34"/>
       <c r="F40" s="3" t="s">
         <v>27</v>
       </c>
@@ -2480,7 +2480,7 @@
       <c r="D41" s="9">
         <v>36</v>
       </c>
-      <c r="E41" s="32"/>
+      <c r="E41" s="34"/>
       <c r="F41" s="3" t="s">
         <v>28</v>
       </c>
@@ -2511,7 +2511,7 @@
       <c r="D42" s="7">
         <v>37</v>
       </c>
-      <c r="E42" s="32"/>
+      <c r="E42" s="34"/>
       <c r="F42" s="5" t="s">
         <v>29</v>
       </c>
@@ -2542,7 +2542,7 @@
       <c r="D43" s="8">
         <v>38</v>
       </c>
-      <c r="E43" s="32"/>
+      <c r="E43" s="34"/>
       <c r="F43" s="4" t="s">
         <v>30</v>
       </c>
@@ -2573,7 +2573,7 @@
       <c r="D44" s="9">
         <v>39</v>
       </c>
-      <c r="E44" s="32"/>
+      <c r="E44" s="34"/>
       <c r="F44" s="3" t="s">
         <v>31</v>
       </c>
@@ -2604,7 +2604,7 @@
       <c r="D45" s="9">
         <v>40</v>
       </c>
-      <c r="E45" s="32"/>
+      <c r="E45" s="34"/>
       <c r="F45" s="3" t="s">
         <v>32</v>
       </c>
@@ -2635,7 +2635,7 @@
       <c r="D46" s="7">
         <v>41</v>
       </c>
-      <c r="E46" s="32"/>
+      <c r="E46" s="34"/>
       <c r="F46" s="5" t="s">
         <v>33</v>
       </c>
@@ -2666,7 +2666,7 @@
       <c r="D47" s="8">
         <v>42</v>
       </c>
-      <c r="E47" s="32"/>
+      <c r="E47" s="34"/>
       <c r="F47" s="4" t="s">
         <v>34</v>
       </c>
@@ -2697,7 +2697,7 @@
       <c r="D48" s="23">
         <v>43</v>
       </c>
-      <c r="E48" s="33"/>
+      <c r="E48" s="35"/>
       <c r="F48" s="22" t="s">
         <v>35</v>
       </c>
@@ -2728,7 +2728,7 @@
       <c r="D49" s="12">
         <v>44</v>
       </c>
-      <c r="E49" s="31" t="s">
+      <c r="E49" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F49" s="11" t="s">
@@ -2761,7 +2761,7 @@
       <c r="D50" s="8">
         <v>45</v>
       </c>
-      <c r="E50" s="32"/>
+      <c r="E50" s="34"/>
       <c r="F50" s="4" t="s">
         <v>15</v>
       </c>
@@ -2792,7 +2792,7 @@
       <c r="D51" s="9">
         <v>46</v>
       </c>
-      <c r="E51" s="32"/>
+      <c r="E51" s="34"/>
       <c r="F51" s="3" t="s">
         <v>16</v>
       </c>
@@ -2823,7 +2823,7 @@
       <c r="D52" s="9">
         <v>47</v>
       </c>
-      <c r="E52" s="32"/>
+      <c r="E52" s="34"/>
       <c r="F52" s="3" t="s">
         <v>17</v>
       </c>
@@ -2854,7 +2854,7 @@
       <c r="D53" s="7">
         <v>48</v>
       </c>
-      <c r="E53" s="32"/>
+      <c r="E53" s="34"/>
       <c r="F53" s="5" t="s">
         <v>18</v>
       </c>
@@ -2885,7 +2885,7 @@
       <c r="D54" s="8">
         <v>49</v>
       </c>
-      <c r="E54" s="32"/>
+      <c r="E54" s="34"/>
       <c r="F54" s="4" t="s">
         <v>19</v>
       </c>
@@ -2916,7 +2916,7 @@
       <c r="D55" s="9">
         <v>50</v>
       </c>
-      <c r="E55" s="32"/>
+      <c r="E55" s="34"/>
       <c r="F55" s="3" t="s">
         <v>20</v>
       </c>
@@ -2947,7 +2947,7 @@
       <c r="D56" s="9">
         <v>51</v>
       </c>
-      <c r="E56" s="32"/>
+      <c r="E56" s="34"/>
       <c r="F56" s="3" t="s">
         <v>21</v>
       </c>
@@ -2978,7 +2978,7 @@
       <c r="D57" s="7">
         <v>52</v>
       </c>
-      <c r="E57" s="32"/>
+      <c r="E57" s="34"/>
       <c r="F57" s="5" t="s">
         <v>22</v>
       </c>
@@ -3009,7 +3009,7 @@
       <c r="D58" s="8">
         <v>53</v>
       </c>
-      <c r="E58" s="32"/>
+      <c r="E58" s="34"/>
       <c r="F58" s="4" t="s">
         <v>23</v>
       </c>
@@ -3040,7 +3040,7 @@
       <c r="D59" s="23">
         <v>54</v>
       </c>
-      <c r="E59" s="33"/>
+      <c r="E59" s="35"/>
       <c r="F59" s="22" t="s">
         <v>24</v>
       </c>
@@ -7310,7 +7310,7 @@
       <c r="D3" s="12">
         <v>0</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="11" t="s">
@@ -7373,7 +7373,7 @@
       <c r="D4" s="8">
         <v>1</v>
       </c>
-      <c r="E4" s="32"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="4" t="s">
         <v>3</v>
       </c>
@@ -7432,7 +7432,7 @@
       <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="3" t="s">
         <v>4</v>
       </c>
@@ -7493,7 +7493,7 @@
       <c r="D6" s="9">
         <v>3</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="3" t="s">
         <v>5</v>
       </c>
@@ -7554,7 +7554,7 @@
       <c r="D7" s="9">
         <v>4</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
@@ -7613,7 +7613,7 @@
       <c r="D8" s="12">
         <v>5</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="33" t="s">
         <v>60</v>
       </c>
       <c r="F8" s="11" t="s">
@@ -7676,7 +7676,7 @@
       <c r="D9" s="8">
         <v>6</v>
       </c>
-      <c r="E9" s="32"/>
+      <c r="E9" s="34"/>
       <c r="F9" s="4" t="s">
         <v>3</v>
       </c>
@@ -7737,7 +7737,7 @@
       <c r="D10" s="9">
         <v>7</v>
       </c>
-      <c r="E10" s="32"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="3" t="s">
         <v>4</v>
       </c>
@@ -7786,7 +7786,7 @@
       <c r="D11" s="9">
         <v>8</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="34"/>
       <c r="F11" s="3" t="s">
         <v>5</v>
       </c>
@@ -7832,7 +7832,7 @@
       <c r="D12" s="9">
         <v>9</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="34"/>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
@@ -9773,7 +9773,7 @@
       <c r="D3" s="12">
         <v>0</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="11" t="s">
@@ -9843,7 +9843,7 @@
       <c r="D4" s="8">
         <v>1</v>
       </c>
-      <c r="E4" s="32"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="4" t="s">
         <v>3</v>
       </c>
@@ -9911,7 +9911,7 @@
       <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="3" t="s">
         <v>4</v>
       </c>
@@ -9979,7 +9979,7 @@
       <c r="D6" s="9">
         <v>3</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="3" t="s">
         <v>5</v>
       </c>
@@ -10047,7 +10047,7 @@
       <c r="D7" s="9">
         <v>4</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
@@ -10113,7 +10113,7 @@
       <c r="D8" s="12">
         <v>5</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="33" t="s">
         <v>60</v>
       </c>
       <c r="F8" s="11" t="s">
@@ -10183,7 +10183,7 @@
       <c r="D9" s="8">
         <v>6</v>
       </c>
-      <c r="E9" s="32"/>
+      <c r="E9" s="34"/>
       <c r="F9" s="4" t="s">
         <v>3</v>
       </c>
@@ -10251,7 +10251,7 @@
       <c r="D10" s="9">
         <v>7</v>
       </c>
-      <c r="E10" s="32"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="3" t="s">
         <v>4</v>
       </c>
@@ -10301,7 +10301,7 @@
       <c r="D11" s="9">
         <v>8</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="34"/>
       <c r="F11" s="3" t="s">
         <v>5</v>
       </c>
@@ -10352,7 +10352,7 @@
       <c r="D12" s="9">
         <v>9</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="34"/>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
@@ -12245,13 +12245,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AA322"/>
+  <dimension ref="B1:AB322"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="10" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R2" sqref="R2:Z9"/>
+      <selection pane="bottomRight" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12262,11 +12262,12 @@
     <col min="10" max="10" width="2.85546875" customWidth="1"/>
     <col min="11" max="19" width="15.7109375" customWidth="1"/>
     <col min="20" max="20" width="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="27" width="15.7109375" customWidth="1"/>
+    <col min="21" max="21" width="20" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="28" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:28" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1">
         <f>K38</f>
         <v>401</v>
@@ -12297,10 +12298,10 @@
         <v>111</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="U1" s="2" t="s">
         <v>70</v>
@@ -12320,9 +12321,9 @@
       <c r="Z1" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="AA1" s="27"/>
-    </row>
-    <row r="2" spans="2:27" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB1" s="27"/>
+    </row>
+    <row r="2" spans="2:28" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>48</v>
       </c>
@@ -12361,11 +12362,11 @@
       <c r="R2" s="2">
         <v>0</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="30">
+        <v>101</v>
+      </c>
+      <c r="T2" s="2">
         <v>201</v>
-      </c>
-      <c r="T2" s="30">
-        <v>101</v>
       </c>
       <c r="U2" s="2">
         <v>301</v>
@@ -12385,9 +12386,9 @@
       <c r="Z2" s="2">
         <v>3</v>
       </c>
-      <c r="AA2" s="2"/>
-    </row>
-    <row r="3" spans="2:27" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AB2" s="2"/>
+    </row>
+    <row r="3" spans="2:28" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10">
         <f>QUOTIENT(D3,5)+1</f>
         <v>1</v>
@@ -12399,7 +12400,7 @@
       <c r="D3" s="12">
         <v>0</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="11" t="s">
@@ -12434,11 +12435,11 @@
       <c r="R3" s="2">
         <v>1</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="30">
+        <v>102</v>
+      </c>
+      <c r="T3" s="2">
         <v>201</v>
-      </c>
-      <c r="T3" s="30">
-        <v>102</v>
       </c>
       <c r="U3" s="2">
         <v>302</v>
@@ -12458,9 +12459,9 @@
       <c r="Z3" s="2">
         <v>3</v>
       </c>
-      <c r="AA3" s="2"/>
-    </row>
-    <row r="4" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB3" s="2"/>
+    </row>
+    <row r="4" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15">
         <f t="shared" ref="B4:B12" si="0">QUOTIENT(D4,5)+1</f>
         <v>1</v>
@@ -12472,7 +12473,7 @@
       <c r="D4" s="8">
         <v>1</v>
       </c>
-      <c r="E4" s="32"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="4" t="s">
         <v>3</v>
       </c>
@@ -12505,11 +12506,11 @@
       <c r="R4" s="2">
         <v>2</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="30">
+        <v>103</v>
+      </c>
+      <c r="T4" s="2">
         <v>201</v>
-      </c>
-      <c r="T4" s="30">
-        <v>103</v>
       </c>
       <c r="U4" s="2">
         <v>303</v>
@@ -12529,9 +12530,9 @@
       <c r="Z4" s="2">
         <v>3</v>
       </c>
-      <c r="AA4" s="2"/>
-    </row>
-    <row r="5" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB4" s="2"/>
+    </row>
+    <row r="5" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="17">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -12543,7 +12544,7 @@
       <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="3" t="s">
         <v>4</v>
       </c>
@@ -12576,11 +12577,11 @@
       <c r="R5" s="2">
         <v>3</v>
       </c>
-      <c r="S5" s="2">
-        <v>202</v>
-      </c>
-      <c r="T5" s="30">
+      <c r="S5" s="30">
         <v>104</v>
+      </c>
+      <c r="T5" s="2">
+        <v>201</v>
       </c>
       <c r="U5" s="2">
         <v>304</v>
@@ -12600,9 +12601,9 @@
       <c r="Z5" s="2">
         <v>3</v>
       </c>
-      <c r="AA5" s="2"/>
-    </row>
-    <row r="6" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB5" s="2"/>
+    </row>
+    <row r="6" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -12614,7 +12615,7 @@
       <c r="D6" s="9">
         <v>3</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="3" t="s">
         <v>5</v>
       </c>
@@ -12647,11 +12648,11 @@
       <c r="R6" s="2">
         <v>4</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6" s="30">
+        <v>101</v>
+      </c>
+      <c r="T6" s="2">
         <v>202</v>
-      </c>
-      <c r="T6" s="30">
-        <v>101</v>
       </c>
       <c r="U6" s="2">
         <v>301</v>
@@ -12671,9 +12672,9 @@
       <c r="Z6" s="2">
         <v>3</v>
       </c>
-      <c r="AA6" s="2"/>
-    </row>
-    <row r="7" spans="2:27" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB6" s="2"/>
+    </row>
+    <row r="7" spans="2:28" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="17">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -12685,7 +12686,7 @@
       <c r="D7" s="9">
         <v>4</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
@@ -12716,11 +12717,11 @@
       <c r="R7" s="2">
         <v>5</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="30">
+        <v>102</v>
+      </c>
+      <c r="T7" s="2">
         <v>202</v>
-      </c>
-      <c r="T7" s="30">
-        <v>102</v>
       </c>
       <c r="U7" s="2">
         <v>302</v>
@@ -12740,9 +12741,9 @@
       <c r="Z7" s="2">
         <v>3</v>
       </c>
-      <c r="AA7" s="2"/>
-    </row>
-    <row r="8" spans="2:27" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AB7" s="2"/>
+    </row>
+    <row r="8" spans="2:28" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -12754,7 +12755,7 @@
       <c r="D8" s="12">
         <v>5</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="33" t="s">
         <v>60</v>
       </c>
       <c r="F8" s="11" t="s">
@@ -12789,11 +12790,11 @@
       <c r="R8" s="2">
         <v>6</v>
       </c>
-      <c r="S8" s="2">
+      <c r="S8" s="30">
+        <v>103</v>
+      </c>
+      <c r="T8" s="2">
         <v>202</v>
-      </c>
-      <c r="T8" s="30">
-        <v>103</v>
       </c>
       <c r="U8" s="2">
         <v>303</v>
@@ -12813,9 +12814,9 @@
       <c r="Z8" s="2">
         <v>3</v>
       </c>
-      <c r="AA8" s="2"/>
-    </row>
-    <row r="9" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB8" s="2"/>
+    </row>
+    <row r="9" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -12827,7 +12828,7 @@
       <c r="D9" s="8">
         <v>6</v>
       </c>
-      <c r="E9" s="32"/>
+      <c r="E9" s="34"/>
       <c r="F9" s="4" t="s">
         <v>3</v>
       </c>
@@ -12860,11 +12861,11 @@
       <c r="R9" s="2">
         <v>7</v>
       </c>
-      <c r="S9" s="2">
+      <c r="S9" s="30">
+        <v>104</v>
+      </c>
+      <c r="T9" s="2">
         <v>202</v>
-      </c>
-      <c r="T9" s="30">
-        <v>104</v>
       </c>
       <c r="U9" s="2">
         <v>304</v>
@@ -12884,9 +12885,9 @@
       <c r="Z9" s="2">
         <v>2</v>
       </c>
-      <c r="AA9" s="2"/>
-    </row>
-    <row r="10" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB9" s="2"/>
+    </row>
+    <row r="10" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="17">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -12898,7 +12899,7 @@
       <c r="D10" s="9">
         <v>7</v>
       </c>
-      <c r="E10" s="32"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="3" t="s">
         <v>4</v>
       </c>
@@ -12919,9 +12920,10 @@
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
-      <c r="AA10" s="25"/>
-    </row>
-    <row r="11" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="25"/>
+    </row>
+    <row r="11" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="17">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -12933,7 +12935,7 @@
       <c r="D11" s="9">
         <v>8</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="34"/>
       <c r="F11" s="3" t="s">
         <v>5</v>
       </c>
@@ -12958,12 +12960,13 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
-      <c r="X11" s="2"/>
+      <c r="W11" s="2"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
-    </row>
-    <row r="12" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB11" s="2"/>
+    </row>
+    <row r="12" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="17">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -12975,7 +12978,7 @@
       <c r="D12" s="9">
         <v>9</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="34"/>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
@@ -13005,8 +13008,9 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
-    </row>
-    <row r="13" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB12" s="2"/>
+    </row>
+    <row r="13" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="28"/>
       <c r="C13" s="28"/>
       <c r="D13" s="29"/>
@@ -13031,8 +13035,9 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
-    </row>
-    <row r="14" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB13" s="2"/>
+    </row>
+    <row r="14" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="28" t="s">
         <v>127</v>
       </c>
@@ -13053,8 +13058,9 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
-    </row>
-    <row r="15" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB14" s="2"/>
+    </row>
+    <row r="15" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
       <c r="D15" s="29" t="s">
@@ -13075,8 +13081,9 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
-    </row>
-    <row r="16" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB15" s="2"/>
+    </row>
+    <row r="16" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="28"/>
       <c r="C16" s="28" t="s">
         <v>128</v>
@@ -13097,8 +13104,9 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
-    </row>
-    <row r="17" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB16" s="2"/>
+    </row>
+    <row r="17" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
       <c r="D17" s="29"/>
@@ -13117,13 +13125,14 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
-    </row>
-    <row r="18" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB17" s="2"/>
+    </row>
+    <row r="18" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="28"/>
       <c r="C18" s="29">
         <v>50</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="32" t="s">
         <v>129</v>
       </c>
       <c r="F18" s="28"/>
@@ -13147,8 +13156,9 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
-    </row>
-    <row r="19" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB18" s="2"/>
+    </row>
+    <row r="19" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="K19" s="2"/>
@@ -13168,17 +13178,18 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
-    </row>
-    <row r="20" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB19" s="2"/>
+    </row>
+    <row r="20" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="W20" s="2"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
-    </row>
-    <row r="21" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB20" s="2"/>
+    </row>
+    <row r="21" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="K21" s="2" t="s">
@@ -13198,25 +13209,26 @@
       </c>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-      <c r="R21" s="34" t="s">
+      <c r="R21" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="S21" s="34" t="s">
+      <c r="S21" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="T21" s="34" t="s">
+      <c r="T21" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="U21" s="34" t="s">
+      <c r="U21" s="31"/>
+      <c r="V21" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="V21" s="2"/>
-      <c r="X21" s="2"/>
+      <c r="W21" s="2"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
-    </row>
-    <row r="22" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB21" s="2"/>
+    </row>
+    <row r="22" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="K22" s="2">
@@ -13250,8 +13262,9 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
-    </row>
-    <row r="23" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB22" s="2"/>
+    </row>
+    <row r="23" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="K23" s="2">
@@ -13285,8 +13298,9 @@
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
-    </row>
-    <row r="24" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB23" s="2"/>
+    </row>
+    <row r="24" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="K24" s="2">
@@ -13320,8 +13334,9 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
-    </row>
-    <row r="25" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB24" s="2"/>
+    </row>
+    <row r="25" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="K25" s="2">
@@ -13355,8 +13370,9 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
-    </row>
-    <row r="26" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB25" s="2"/>
+    </row>
+    <row r="26" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="K26" s="2"/>
@@ -13380,8 +13396,9 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
-    </row>
-    <row r="27" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB26" s="2"/>
+    </row>
+    <row r="27" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="K27" s="2" t="s">
@@ -13413,8 +13430,9 @@
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
-    </row>
-    <row r="28" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB27" s="2"/>
+    </row>
+    <row r="28" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="K28" s="2">
@@ -13441,8 +13459,9 @@
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
-    </row>
-    <row r="29" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W28" s="2"/>
+    </row>
+    <row r="29" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="K29" s="2">
@@ -13469,8 +13488,9 @@
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
-    </row>
-    <row r="30" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W29" s="2"/>
+    </row>
+    <row r="30" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="K30" s="2"/>
@@ -13487,8 +13507,9 @@
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
-    </row>
-    <row r="31" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W30" s="2"/>
+    </row>
+    <row r="31" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="K31" s="2" t="s">
@@ -13511,8 +13532,9 @@
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
-    </row>
-    <row r="32" spans="2:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W31" s="2"/>
+    </row>
+    <row r="32" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="K32" s="2">
@@ -13535,8 +13557,9 @@
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
-    </row>
-    <row r="33" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W32" s="2"/>
+    </row>
+    <row r="33" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="K33" s="2">
@@ -13559,8 +13582,9 @@
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
-    </row>
-    <row r="34" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W33" s="2"/>
+    </row>
+    <row r="34" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="K34" s="2">
@@ -13583,8 +13607,9 @@
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
-    </row>
-    <row r="35" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W34" s="2"/>
+    </row>
+    <row r="35" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="K35" s="2">
@@ -13607,8 +13632,9 @@
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
-    </row>
-    <row r="36" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W35" s="2"/>
+    </row>
+    <row r="36" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="K36" s="2"/>
@@ -13625,8 +13651,9 @@
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
-    </row>
-    <row r="37" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W36" s="2"/>
+    </row>
+    <row r="37" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="K37" s="2" t="s">
@@ -13651,8 +13678,9 @@
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
-    </row>
-    <row r="38" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W37" s="2"/>
+    </row>
+    <row r="38" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="K38" s="2">
@@ -13677,8 +13705,9 @@
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
-    </row>
-    <row r="39" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W38" s="2"/>
+    </row>
+    <row r="39" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="K39" s="2">
@@ -13703,8 +13732,9 @@
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
-    </row>
-    <row r="40" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W39" s="2"/>
+    </row>
+    <row r="40" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="K40" s="2"/>
@@ -13721,57 +13751,58 @@
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
-    </row>
-    <row r="41" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W40" s="2"/>
+    </row>
+    <row r="41" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="R41" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="R42" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="R43" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="R44" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="R45" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="R46" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="R47" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="8:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="R48" s="2">
@@ -14949,14 +14980,14 @@
     <mergeCell ref="E8:E12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="T2" location="'Sheet3 (3)'!K22" display="'Sheet3 (3)'!K22"/>
-    <hyperlink ref="T3" location="'Sheet3 (3)'!K23" display="'Sheet3 (3)'!K23"/>
-    <hyperlink ref="T4" location="'Sheet3 (3)'!K24" display="'Sheet3 (3)'!K24"/>
-    <hyperlink ref="T5" location="'Sheet3 (3)'!K25" display="'Sheet3 (3)'!K25"/>
-    <hyperlink ref="T6" location="'Sheet3 (3)'!K22" display="'Sheet3 (3)'!K22"/>
-    <hyperlink ref="T7" location="'Sheet3 (3)'!K23" display="'Sheet3 (3)'!K23"/>
-    <hyperlink ref="T8" location="'Sheet3 (3)'!K24" display="'Sheet3 (3)'!K24"/>
-    <hyperlink ref="T9" location="'Sheet3 (3)'!K25" display="'Sheet3 (3)'!K25"/>
+    <hyperlink ref="S2" location="'Sheet3 (3)'!K22" display="'Sheet3 (3)'!K22"/>
+    <hyperlink ref="S3" location="'Sheet3 (3)'!K23" display="'Sheet3 (3)'!K23"/>
+    <hyperlink ref="S4" location="'Sheet3 (3)'!K24" display="'Sheet3 (3)'!K24"/>
+    <hyperlink ref="S5" location="'Sheet3 (3)'!K25" display="'Sheet3 (3)'!K25"/>
+    <hyperlink ref="S6" location="'Sheet3 (3)'!K22" display="'Sheet3 (3)'!K22"/>
+    <hyperlink ref="S7" location="'Sheet3 (3)'!K23" display="'Sheet3 (3)'!K23"/>
+    <hyperlink ref="S8" location="'Sheet3 (3)'!K24" display="'Sheet3 (3)'!K24"/>
+    <hyperlink ref="S9" location="'Sheet3 (3)'!K25" display="'Sheet3 (3)'!K25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added the schedules object
</commit_message>
<xml_diff>
--- a/csv/VisualPlotting.xlsx
+++ b/csv/VisualPlotting.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet3 (2)" sheetId="5" r:id="rId2"/>
     <sheet name="Sheet3 (3)" sheetId="6" r:id="rId3"/>
     <sheet name="Sheet3 (4)" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet3 (5)" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="130">
   <si>
     <t>Room 1</t>
   </si>
@@ -12247,11 +12248,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AB322"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="10" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="10" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q9" sqref="Q9"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12356,7 +12357,7 @@
       </c>
       <c r="O2" s="2"/>
       <c r="P2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2">
@@ -12384,7 +12385,7 @@
         <v>1</v>
       </c>
       <c r="Z2" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB2" s="2"/>
     </row>
@@ -12429,7 +12430,7 @@
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2">
@@ -12500,7 +12501,7 @@
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="2">
@@ -12571,7 +12572,7 @@
       </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="2">
@@ -12599,7 +12600,7 @@
         <v>1</v>
       </c>
       <c r="Z5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB5" s="2"/>
     </row>
@@ -12642,7 +12643,7 @@
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="2">
@@ -12670,7 +12671,7 @@
         <v>1</v>
       </c>
       <c r="Z6" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB6" s="2"/>
     </row>
@@ -12711,7 +12712,7 @@
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2">
@@ -12784,7 +12785,7 @@
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2">
@@ -12855,7 +12856,7 @@
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="2">
@@ -13219,10 +13220,9 @@
         <v>124</v>
       </c>
       <c r="U21" s="31"/>
-      <c r="V21" s="31" t="s">
+      <c r="W21" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="W21" s="2"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
@@ -13257,7 +13257,9 @@
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
+      <c r="W22" s="2">
+        <v>0</v>
+      </c>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
@@ -13293,7 +13295,9 @@
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
+      <c r="W23" s="2">
+        <v>1</v>
+      </c>
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
@@ -13329,7 +13333,9 @@
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
+      <c r="W24" s="2">
+        <v>2</v>
+      </c>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
@@ -13365,7 +13371,9 @@
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
+      <c r="W25" s="2">
+        <v>3</v>
+      </c>
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
@@ -13391,7 +13399,9 @@
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
-      <c r="W26" s="2"/>
+      <c r="W26" s="2">
+        <v>4</v>
+      </c>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
@@ -13425,7 +13435,9 @@
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
-      <c r="W27" s="2"/>
+      <c r="W27" s="2">
+        <v>5</v>
+      </c>
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
@@ -13459,7 +13471,9 @@
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
-      <c r="W28" s="2"/>
+      <c r="W28" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="29" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H29" s="2"/>
@@ -13488,7 +13502,9 @@
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
+      <c r="W29" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="30" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H30" s="2"/>
@@ -13507,7 +13523,9 @@
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
-      <c r="W30" s="2"/>
+      <c r="W30" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="31" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H31" s="2"/>
@@ -13532,7 +13550,2779 @@
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
-      <c r="W31" s="2"/>
+      <c r="W31" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="K32" s="2">
+        <v>301</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2">
+        <v>10</v>
+      </c>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+    </row>
+    <row r="33" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="K33" s="2">
+        <v>302</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2">
+        <v>11</v>
+      </c>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+    </row>
+    <row r="34" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="K34" s="2">
+        <v>303</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2">
+        <v>12</v>
+      </c>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+    </row>
+    <row r="35" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="K35" s="2">
+        <v>304</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2">
+        <v>13</v>
+      </c>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+    </row>
+    <row r="36" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2">
+        <v>14</v>
+      </c>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+    </row>
+    <row r="37" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="K37" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2">
+        <v>15</v>
+      </c>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+    </row>
+    <row r="38" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="K38" s="2">
+        <v>401</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2">
+        <v>16</v>
+      </c>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+    </row>
+    <row r="39" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="K39" s="2">
+        <v>402</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2">
+        <v>17</v>
+      </c>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+    </row>
+    <row r="40" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2">
+        <v>18</v>
+      </c>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+    </row>
+    <row r="41" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="R41" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="R42" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="R43" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="R44" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="R45" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="R46" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="R47" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="8:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="R48" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="R49" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="R50" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="R51" s="2"/>
+    </row>
+    <row r="52" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="R52" s="2"/>
+    </row>
+    <row r="53" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="R53" s="2"/>
+    </row>
+    <row r="54" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="R54" s="2"/>
+    </row>
+    <row r="55" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="R55" s="2"/>
+    </row>
+    <row r="56" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="R56" s="2"/>
+    </row>
+    <row r="57" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="R57" s="2"/>
+    </row>
+    <row r="58" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="R58" s="2"/>
+    </row>
+    <row r="59" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="R59" s="2"/>
+    </row>
+    <row r="60" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="R60" s="2"/>
+    </row>
+    <row r="61" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="R61" s="2"/>
+    </row>
+    <row r="62" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="R62" s="2"/>
+    </row>
+    <row r="63" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="R63" s="2"/>
+    </row>
+    <row r="64" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="R64" s="2"/>
+    </row>
+    <row r="65" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="R65" s="2"/>
+    </row>
+    <row r="66" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="R66" s="2"/>
+    </row>
+    <row r="67" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="R67" s="2"/>
+    </row>
+    <row r="68" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="R68" s="2"/>
+    </row>
+    <row r="69" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="R69" s="2"/>
+    </row>
+    <row r="70" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="R70" s="2"/>
+    </row>
+    <row r="71" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="R71" s="2"/>
+    </row>
+    <row r="72" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="R72" s="2"/>
+    </row>
+    <row r="73" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="R73" s="2"/>
+    </row>
+    <row r="74" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="R74" s="2"/>
+    </row>
+    <row r="75" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="R75" s="2"/>
+    </row>
+    <row r="76" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="R76" s="2"/>
+    </row>
+    <row r="77" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="R77" s="2"/>
+    </row>
+    <row r="78" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="R78" s="2"/>
+    </row>
+    <row r="79" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
+      <c r="R79" s="2"/>
+    </row>
+    <row r="80" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="R80" s="2"/>
+    </row>
+    <row r="81" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="R81" s="2"/>
+    </row>
+    <row r="82" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="R82" s="2"/>
+    </row>
+    <row r="83" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="R83" s="2"/>
+    </row>
+    <row r="84" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+      <c r="R84" s="2"/>
+    </row>
+    <row r="85" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="R85" s="2"/>
+    </row>
+    <row r="86" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+      <c r="R86" s="2"/>
+    </row>
+    <row r="87" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="R87" s="2"/>
+    </row>
+    <row r="88" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
+      <c r="R88" s="2"/>
+    </row>
+    <row r="89" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+      <c r="R89" s="2"/>
+    </row>
+    <row r="90" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+      <c r="R90" s="2"/>
+    </row>
+    <row r="91" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+      <c r="R91" s="2"/>
+    </row>
+    <row r="92" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="R92" s="2"/>
+    </row>
+    <row r="93" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+      <c r="R93" s="2"/>
+    </row>
+    <row r="94" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
+      <c r="R94" s="2"/>
+    </row>
+    <row r="95" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+      <c r="R95" s="2"/>
+    </row>
+    <row r="96" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
+      <c r="R96" s="2"/>
+    </row>
+    <row r="97" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
+      <c r="R97" s="2"/>
+    </row>
+    <row r="98" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
+      <c r="R98" s="2"/>
+    </row>
+    <row r="99" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
+      <c r="R99" s="2"/>
+    </row>
+    <row r="100" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
+      <c r="R100" s="2"/>
+    </row>
+    <row r="101" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="R101" s="2"/>
+    </row>
+    <row r="102" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="R102" s="2"/>
+    </row>
+    <row r="103" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+      <c r="R103" s="2"/>
+    </row>
+    <row r="104" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+      <c r="R104" s="2"/>
+    </row>
+    <row r="105" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="R105" s="2"/>
+    </row>
+    <row r="106" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="R106" s="2"/>
+    </row>
+    <row r="107" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
+      <c r="R107" s="2"/>
+    </row>
+    <row r="108" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="R108" s="2"/>
+    </row>
+    <row r="109" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="R109" s="2"/>
+    </row>
+    <row r="110" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
+      <c r="R110" s="2"/>
+    </row>
+    <row r="111" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+      <c r="R111" s="2"/>
+    </row>
+    <row r="112" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="R112" s="2"/>
+    </row>
+    <row r="113" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+      <c r="R113" s="2"/>
+    </row>
+    <row r="114" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+    </row>
+    <row r="115" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+    </row>
+    <row r="116" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+    </row>
+    <row r="117" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
+    </row>
+    <row r="118" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
+    </row>
+    <row r="119" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H119" s="2"/>
+      <c r="I119" s="2"/>
+    </row>
+    <row r="120" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
+    </row>
+    <row r="121" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
+    </row>
+    <row r="122" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
+    </row>
+    <row r="123" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H123" s="2"/>
+      <c r="I123" s="2"/>
+    </row>
+    <row r="124" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
+    </row>
+    <row r="125" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H125" s="2"/>
+      <c r="I125" s="2"/>
+    </row>
+    <row r="126" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H126" s="2"/>
+      <c r="I126" s="2"/>
+    </row>
+    <row r="127" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H127" s="2"/>
+      <c r="I127" s="2"/>
+    </row>
+    <row r="128" spans="8:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H128" s="2"/>
+      <c r="I128" s="2"/>
+    </row>
+    <row r="129" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H129" s="2"/>
+      <c r="I129" s="2"/>
+    </row>
+    <row r="130" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H130" s="2"/>
+      <c r="I130" s="2"/>
+    </row>
+    <row r="131" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H131" s="2"/>
+      <c r="I131" s="2"/>
+    </row>
+    <row r="132" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H132" s="2"/>
+      <c r="I132" s="2"/>
+    </row>
+    <row r="133" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H133" s="2"/>
+      <c r="I133" s="2"/>
+    </row>
+    <row r="134" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H134" s="2"/>
+      <c r="I134" s="2"/>
+    </row>
+    <row r="135" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H135" s="2"/>
+      <c r="I135" s="2"/>
+    </row>
+    <row r="136" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H136" s="2"/>
+      <c r="I136" s="2"/>
+    </row>
+    <row r="137" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H137" s="2"/>
+      <c r="I137" s="2"/>
+    </row>
+    <row r="138" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H138" s="2"/>
+      <c r="I138" s="2"/>
+    </row>
+    <row r="139" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H139" s="2"/>
+      <c r="I139" s="2"/>
+    </row>
+    <row r="140" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H140" s="2"/>
+      <c r="I140" s="2"/>
+    </row>
+    <row r="141" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H141" s="2"/>
+      <c r="I141" s="2"/>
+    </row>
+    <row r="142" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H142" s="2"/>
+      <c r="I142" s="2"/>
+    </row>
+    <row r="143" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H143" s="2"/>
+      <c r="I143" s="2"/>
+    </row>
+    <row r="144" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H144" s="2"/>
+      <c r="I144" s="2"/>
+    </row>
+    <row r="145" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H145" s="2"/>
+      <c r="I145" s="2"/>
+    </row>
+    <row r="146" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H146" s="2"/>
+      <c r="I146" s="2"/>
+    </row>
+    <row r="147" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H147" s="2"/>
+      <c r="I147" s="2"/>
+    </row>
+    <row r="148" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H148" s="2"/>
+      <c r="I148" s="2"/>
+    </row>
+    <row r="149" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H149" s="2"/>
+      <c r="I149" s="2"/>
+    </row>
+    <row r="150" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H150" s="2"/>
+      <c r="I150" s="2"/>
+    </row>
+    <row r="151" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H151" s="2"/>
+      <c r="I151" s="2"/>
+    </row>
+    <row r="152" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H152" s="2"/>
+      <c r="I152" s="2"/>
+    </row>
+    <row r="153" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H153" s="2"/>
+      <c r="I153" s="2"/>
+    </row>
+    <row r="154" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H154" s="2"/>
+      <c r="I154" s="2"/>
+    </row>
+    <row r="155" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H155" s="2"/>
+      <c r="I155" s="2"/>
+    </row>
+    <row r="156" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H156" s="2"/>
+      <c r="I156" s="2"/>
+    </row>
+    <row r="157" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H157" s="2"/>
+      <c r="I157" s="2"/>
+    </row>
+    <row r="158" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H158" s="2"/>
+      <c r="I158" s="2"/>
+    </row>
+    <row r="159" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H159" s="2"/>
+      <c r="I159" s="2"/>
+    </row>
+    <row r="160" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H160" s="2"/>
+      <c r="I160" s="2"/>
+    </row>
+    <row r="161" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H161" s="2"/>
+      <c r="I161" s="2"/>
+    </row>
+    <row r="162" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H162" s="2"/>
+      <c r="I162" s="2"/>
+    </row>
+    <row r="163" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H163" s="2"/>
+      <c r="I163" s="2"/>
+    </row>
+    <row r="164" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H164" s="2"/>
+      <c r="I164" s="2"/>
+    </row>
+    <row r="165" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H165" s="2"/>
+      <c r="I165" s="2"/>
+    </row>
+    <row r="166" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H166" s="2"/>
+      <c r="I166" s="2"/>
+    </row>
+    <row r="167" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H167" s="2"/>
+      <c r="I167" s="2"/>
+    </row>
+    <row r="168" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H168" s="2"/>
+      <c r="I168" s="2"/>
+    </row>
+    <row r="169" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H169" s="2"/>
+      <c r="I169" s="2"/>
+    </row>
+    <row r="170" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H170" s="2"/>
+      <c r="I170" s="2"/>
+    </row>
+    <row r="171" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H171" s="2"/>
+      <c r="I171" s="2"/>
+    </row>
+    <row r="172" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H172" s="2"/>
+      <c r="I172" s="2"/>
+    </row>
+    <row r="173" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H173" s="2"/>
+      <c r="I173" s="2"/>
+    </row>
+    <row r="174" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H174" s="2"/>
+      <c r="I174" s="2"/>
+    </row>
+    <row r="175" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H175" s="2"/>
+      <c r="I175" s="2"/>
+    </row>
+    <row r="176" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H176" s="2"/>
+      <c r="I176" s="2"/>
+    </row>
+    <row r="177" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H177" s="2"/>
+      <c r="I177" s="2"/>
+    </row>
+    <row r="178" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H178" s="2"/>
+      <c r="I178" s="2"/>
+    </row>
+    <row r="179" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H179" s="2"/>
+      <c r="I179" s="2"/>
+    </row>
+    <row r="180" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H180" s="2"/>
+      <c r="I180" s="2"/>
+    </row>
+    <row r="181" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H181" s="2"/>
+      <c r="I181" s="2"/>
+    </row>
+    <row r="182" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H182" s="2"/>
+      <c r="I182" s="2"/>
+    </row>
+    <row r="183" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H183" s="2"/>
+      <c r="I183" s="2"/>
+    </row>
+    <row r="184" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H184" s="2"/>
+      <c r="I184" s="2"/>
+    </row>
+    <row r="185" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H185" s="2"/>
+      <c r="I185" s="2"/>
+    </row>
+    <row r="186" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H186" s="2"/>
+      <c r="I186" s="2"/>
+    </row>
+    <row r="187" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H187" s="2"/>
+      <c r="I187" s="2"/>
+    </row>
+    <row r="188" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H188" s="2"/>
+      <c r="I188" s="2"/>
+    </row>
+    <row r="189" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H189" s="2"/>
+      <c r="I189" s="2"/>
+    </row>
+    <row r="190" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H190" s="2"/>
+      <c r="I190" s="2"/>
+    </row>
+    <row r="191" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H191" s="2"/>
+      <c r="I191" s="2"/>
+    </row>
+    <row r="192" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H192" s="2"/>
+      <c r="I192" s="2"/>
+    </row>
+    <row r="193" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H193" s="2"/>
+      <c r="I193" s="2"/>
+    </row>
+    <row r="194" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H194" s="2"/>
+      <c r="I194" s="2"/>
+    </row>
+    <row r="195" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H195" s="2"/>
+      <c r="I195" s="2"/>
+    </row>
+    <row r="196" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H196" s="2"/>
+      <c r="I196" s="2"/>
+    </row>
+    <row r="197" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H197" s="2"/>
+      <c r="I197" s="2"/>
+    </row>
+    <row r="198" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H198" s="2"/>
+      <c r="I198" s="2"/>
+    </row>
+    <row r="199" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H199" s="2"/>
+      <c r="I199" s="2"/>
+    </row>
+    <row r="200" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H200" s="2"/>
+      <c r="I200" s="2"/>
+    </row>
+    <row r="201" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H201" s="2"/>
+      <c r="I201" s="2"/>
+    </row>
+    <row r="202" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H202" s="2"/>
+      <c r="I202" s="2"/>
+    </row>
+    <row r="203" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H203" s="2"/>
+      <c r="I203" s="2"/>
+    </row>
+    <row r="204" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H204" s="2"/>
+      <c r="I204" s="2"/>
+    </row>
+    <row r="205" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H205" s="2"/>
+      <c r="I205" s="2"/>
+    </row>
+    <row r="206" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H206" s="2"/>
+      <c r="I206" s="2"/>
+    </row>
+    <row r="207" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H207" s="2"/>
+      <c r="I207" s="2"/>
+    </row>
+    <row r="208" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H208" s="2"/>
+      <c r="I208" s="2"/>
+    </row>
+    <row r="209" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H209" s="2"/>
+      <c r="I209" s="2"/>
+    </row>
+    <row r="210" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H210" s="2"/>
+      <c r="I210" s="2"/>
+    </row>
+    <row r="211" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H211" s="2"/>
+      <c r="I211" s="2"/>
+    </row>
+    <row r="212" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H212" s="2"/>
+      <c r="I212" s="2"/>
+    </row>
+    <row r="213" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H213" s="2"/>
+      <c r="I213" s="2"/>
+    </row>
+    <row r="214" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H214" s="2"/>
+      <c r="I214" s="2"/>
+    </row>
+    <row r="215" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H215" s="2"/>
+      <c r="I215" s="2"/>
+    </row>
+    <row r="216" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H216" s="2"/>
+      <c r="I216" s="2"/>
+    </row>
+    <row r="217" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H217" s="2"/>
+      <c r="I217" s="2"/>
+    </row>
+    <row r="218" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H218" s="2"/>
+      <c r="I218" s="2"/>
+    </row>
+    <row r="219" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H219" s="2"/>
+      <c r="I219" s="2"/>
+    </row>
+    <row r="220" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H220" s="2"/>
+      <c r="I220" s="2"/>
+    </row>
+    <row r="221" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H221" s="2"/>
+      <c r="I221" s="2"/>
+    </row>
+    <row r="222" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H222" s="2"/>
+      <c r="I222" s="2"/>
+    </row>
+    <row r="223" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H223" s="2"/>
+      <c r="I223" s="2"/>
+    </row>
+    <row r="224" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H224" s="2"/>
+      <c r="I224" s="2"/>
+    </row>
+    <row r="225" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H225" s="2"/>
+      <c r="I225" s="2"/>
+    </row>
+    <row r="226" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H226" s="2"/>
+      <c r="I226" s="2"/>
+    </row>
+    <row r="227" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H227" s="2"/>
+      <c r="I227" s="2"/>
+    </row>
+    <row r="228" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H228" s="2"/>
+      <c r="I228" s="2"/>
+    </row>
+    <row r="229" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H229" s="2"/>
+      <c r="I229" s="2"/>
+    </row>
+    <row r="230" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H230" s="2"/>
+      <c r="I230" s="2"/>
+    </row>
+    <row r="231" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H231" s="2"/>
+      <c r="I231" s="2"/>
+    </row>
+    <row r="232" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H232" s="2"/>
+      <c r="I232" s="2"/>
+    </row>
+    <row r="233" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H233" s="2"/>
+      <c r="I233" s="2"/>
+    </row>
+    <row r="234" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H234" s="2"/>
+      <c r="I234" s="2"/>
+    </row>
+    <row r="235" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H235" s="2"/>
+      <c r="I235" s="2"/>
+    </row>
+    <row r="236" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H236" s="2"/>
+      <c r="I236" s="2"/>
+    </row>
+    <row r="237" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H237" s="2"/>
+      <c r="I237" s="2"/>
+    </row>
+    <row r="238" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H238" s="2"/>
+      <c r="I238" s="2"/>
+    </row>
+    <row r="239" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H239" s="2"/>
+      <c r="I239" s="2"/>
+    </row>
+    <row r="240" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H240" s="2"/>
+      <c r="I240" s="2"/>
+    </row>
+    <row r="241" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H241" s="2"/>
+      <c r="I241" s="2"/>
+    </row>
+    <row r="242" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H242" s="2"/>
+      <c r="I242" s="2"/>
+    </row>
+    <row r="243" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H243" s="2"/>
+      <c r="I243" s="2"/>
+    </row>
+    <row r="244" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H244" s="2"/>
+      <c r="I244" s="2"/>
+    </row>
+    <row r="245" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H245" s="2"/>
+      <c r="I245" s="2"/>
+    </row>
+    <row r="246" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H246" s="2"/>
+      <c r="I246" s="2"/>
+    </row>
+    <row r="247" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H247" s="2"/>
+      <c r="I247" s="2"/>
+    </row>
+    <row r="248" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H248" s="2"/>
+      <c r="I248" s="2"/>
+    </row>
+    <row r="249" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H249" s="2"/>
+      <c r="I249" s="2"/>
+    </row>
+    <row r="250" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H250" s="2"/>
+      <c r="I250" s="2"/>
+    </row>
+    <row r="251" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H251" s="2"/>
+      <c r="I251" s="2"/>
+    </row>
+    <row r="252" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H252" s="2"/>
+      <c r="I252" s="2"/>
+    </row>
+    <row r="253" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H253" s="2"/>
+      <c r="I253" s="2"/>
+    </row>
+    <row r="254" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H254" s="2"/>
+      <c r="I254" s="2"/>
+    </row>
+    <row r="255" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H255" s="2"/>
+      <c r="I255" s="2"/>
+    </row>
+    <row r="256" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H256" s="2"/>
+      <c r="I256" s="2"/>
+    </row>
+    <row r="257" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H257" s="2"/>
+      <c r="I257" s="2"/>
+    </row>
+    <row r="258" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H258" s="2"/>
+      <c r="I258" s="2"/>
+    </row>
+    <row r="259" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H259" s="2"/>
+      <c r="I259" s="2"/>
+    </row>
+    <row r="260" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H260" s="2"/>
+      <c r="I260" s="2"/>
+    </row>
+    <row r="261" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H261" s="2"/>
+      <c r="I261" s="2"/>
+    </row>
+    <row r="262" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H262" s="2"/>
+      <c r="I262" s="2"/>
+    </row>
+    <row r="263" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H263" s="2"/>
+      <c r="I263" s="2"/>
+    </row>
+    <row r="264" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H264" s="2"/>
+      <c r="I264" s="2"/>
+    </row>
+    <row r="265" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H265" s="2"/>
+      <c r="I265" s="2"/>
+    </row>
+    <row r="266" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H266" s="2"/>
+      <c r="I266" s="2"/>
+    </row>
+    <row r="267" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H267" s="2"/>
+      <c r="I267" s="2"/>
+    </row>
+    <row r="268" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H268" s="2"/>
+      <c r="I268" s="2"/>
+    </row>
+    <row r="269" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H269" s="2"/>
+      <c r="I269" s="2"/>
+    </row>
+    <row r="270" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H270" s="2"/>
+      <c r="I270" s="2"/>
+    </row>
+    <row r="271" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H271" s="2"/>
+      <c r="I271" s="2"/>
+    </row>
+    <row r="272" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H272" s="2"/>
+      <c r="I272" s="2"/>
+    </row>
+    <row r="273" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H273" s="2"/>
+      <c r="I273" s="2"/>
+    </row>
+    <row r="274" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H274" s="2"/>
+      <c r="I274" s="2"/>
+    </row>
+    <row r="275" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H275" s="2"/>
+      <c r="I275" s="2"/>
+    </row>
+    <row r="276" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H276" s="2"/>
+      <c r="I276" s="2"/>
+    </row>
+    <row r="277" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H277" s="2"/>
+      <c r="I277" s="2"/>
+    </row>
+    <row r="278" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H278" s="2"/>
+      <c r="I278" s="2"/>
+    </row>
+    <row r="279" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H279" s="2"/>
+      <c r="I279" s="2"/>
+    </row>
+    <row r="280" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H280" s="2"/>
+      <c r="I280" s="2"/>
+    </row>
+    <row r="281" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H281" s="2"/>
+      <c r="I281" s="2"/>
+    </row>
+    <row r="282" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H282" s="2"/>
+      <c r="I282" s="2"/>
+    </row>
+    <row r="283" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H283" s="2"/>
+      <c r="I283" s="2"/>
+    </row>
+    <row r="284" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H284" s="2"/>
+      <c r="I284" s="2"/>
+    </row>
+    <row r="285" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H285" s="2"/>
+      <c r="I285" s="2"/>
+    </row>
+    <row r="286" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H286" s="2"/>
+      <c r="I286" s="2"/>
+    </row>
+    <row r="287" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H287" s="2"/>
+      <c r="I287" s="2"/>
+    </row>
+    <row r="288" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H288" s="2"/>
+      <c r="I288" s="2"/>
+    </row>
+    <row r="289" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H289" s="2"/>
+      <c r="I289" s="2"/>
+    </row>
+    <row r="290" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H290" s="2"/>
+      <c r="I290" s="2"/>
+    </row>
+    <row r="291" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H291" s="2"/>
+      <c r="I291" s="2"/>
+    </row>
+    <row r="292" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H292" s="2"/>
+      <c r="I292" s="2"/>
+    </row>
+    <row r="293" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H293" s="2"/>
+      <c r="I293" s="2"/>
+    </row>
+    <row r="294" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H294" s="2"/>
+      <c r="I294" s="2"/>
+    </row>
+    <row r="295" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H295" s="2"/>
+      <c r="I295" s="2"/>
+    </row>
+    <row r="296" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H296" s="2"/>
+      <c r="I296" s="2"/>
+    </row>
+    <row r="297" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H297" s="2"/>
+      <c r="I297" s="2"/>
+    </row>
+    <row r="298" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H298" s="2"/>
+      <c r="I298" s="2"/>
+    </row>
+    <row r="299" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H299" s="2"/>
+      <c r="I299" s="2"/>
+    </row>
+    <row r="300" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H300" s="2"/>
+      <c r="I300" s="2"/>
+    </row>
+    <row r="301" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H301" s="2"/>
+      <c r="I301" s="2"/>
+    </row>
+    <row r="302" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H302" s="2"/>
+      <c r="I302" s="2"/>
+    </row>
+    <row r="303" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H303" s="2"/>
+      <c r="I303" s="2"/>
+    </row>
+    <row r="304" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H304" s="2"/>
+      <c r="I304" s="2"/>
+    </row>
+    <row r="305" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H305" s="2"/>
+      <c r="I305" s="2"/>
+    </row>
+    <row r="306" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H306" s="2"/>
+      <c r="I306" s="2"/>
+    </row>
+    <row r="307" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H307" s="2"/>
+      <c r="I307" s="2"/>
+    </row>
+    <row r="308" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H308" s="2"/>
+      <c r="I308" s="2"/>
+    </row>
+    <row r="309" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H309" s="2"/>
+      <c r="I309" s="2"/>
+    </row>
+    <row r="310" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H310" s="2"/>
+      <c r="I310" s="2"/>
+    </row>
+    <row r="311" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H311" s="2"/>
+      <c r="I311" s="2"/>
+    </row>
+    <row r="312" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H312" s="2"/>
+      <c r="I312" s="2"/>
+    </row>
+    <row r="313" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H313" s="2"/>
+      <c r="I313" s="2"/>
+    </row>
+    <row r="314" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H314" s="2"/>
+      <c r="I314" s="2"/>
+    </row>
+    <row r="315" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H315" s="2"/>
+      <c r="I315" s="2"/>
+    </row>
+    <row r="316" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H316" s="2"/>
+      <c r="I316" s="2"/>
+    </row>
+    <row r="317" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H317" s="2"/>
+      <c r="I317" s="2"/>
+    </row>
+    <row r="318" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H318" s="2"/>
+      <c r="I318" s="2"/>
+    </row>
+    <row r="319" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H319" s="2"/>
+      <c r="I319" s="2"/>
+    </row>
+    <row r="320" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H320" s="2"/>
+      <c r="I320" s="2"/>
+    </row>
+    <row r="321" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H321" s="2"/>
+      <c r="I321" s="2"/>
+    </row>
+    <row r="322" spans="8:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H322" s="2"/>
+      <c r="I322" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E3:E7"/>
+    <mergeCell ref="E8:E12"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="S2" location="'Sheet3 (3)'!K22" display="'Sheet3 (3)'!K22"/>
+    <hyperlink ref="S3" location="'Sheet3 (3)'!K23" display="'Sheet3 (3)'!K23"/>
+    <hyperlink ref="S4" location="'Sheet3 (3)'!K24" display="'Sheet3 (3)'!K24"/>
+    <hyperlink ref="S5" location="'Sheet3 (3)'!K25" display="'Sheet3 (3)'!K25"/>
+    <hyperlink ref="S6" location="'Sheet3 (3)'!K22" display="'Sheet3 (3)'!K22"/>
+    <hyperlink ref="S7" location="'Sheet3 (3)'!K23" display="'Sheet3 (3)'!K23"/>
+    <hyperlink ref="S8" location="'Sheet3 (3)'!K24" display="'Sheet3 (3)'!K24"/>
+    <hyperlink ref="S9" location="'Sheet3 (3)'!K25" display="'Sheet3 (3)'!K25"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AB322"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="10" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" customWidth="1"/>
+    <col min="11" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="28" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:28" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1">
+        <f>K38</f>
+        <v>401</v>
+      </c>
+      <c r="I1">
+        <v>402</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V1" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="W1" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="X1" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y1" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z1" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB1" s="27"/>
+    </row>
+    <row r="2" spans="2:28" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="str">
+        <f>L38</f>
+        <v>Room 1</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>101</v>
+      </c>
+      <c r="M2" s="2">
+        <v>201</v>
+      </c>
+      <c r="N2" s="2">
+        <v>301</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="30">
+        <v>101</v>
+      </c>
+      <c r="T2" s="2">
+        <v>201</v>
+      </c>
+      <c r="U2" s="2">
+        <v>301</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W2" s="2">
+        <v>1</v>
+      </c>
+      <c r="X2" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="2"/>
+    </row>
+    <row r="3" spans="2:28" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="10">
+        <f>QUOTIENT(D3,5)+1</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="11">
+        <f>MOD(D3,5)+1</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="11">
+        <v>101</v>
+      </c>
+      <c r="H3" s="12">
+        <v>0</v>
+      </c>
+      <c r="I3" s="14">
+        <v>7</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <v>102</v>
+      </c>
+      <c r="M3" s="2">
+        <v>201</v>
+      </c>
+      <c r="N3" s="2">
+        <v>302</v>
+      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2">
+        <v>1</v>
+      </c>
+      <c r="S3" s="30">
+        <v>102</v>
+      </c>
+      <c r="T3" s="2">
+        <v>201</v>
+      </c>
+      <c r="U3" s="2">
+        <v>302</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W3" s="2">
+        <v>1</v>
+      </c>
+      <c r="X3" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB3" s="2"/>
+    </row>
+    <row r="4" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15">
+        <f t="shared" ref="B4:B12" si="0">QUOTIENT(D4,5)+1</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" ref="C4:C12" si="1">MOD(D4,5)+1</f>
+        <v>2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="34"/>
+      <c r="F4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="4">
+        <v>102</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0</v>
+      </c>
+      <c r="I4" s="16">
+        <v>7</v>
+      </c>
+      <c r="K4" s="2">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2">
+        <v>103</v>
+      </c>
+      <c r="M4" s="2">
+        <v>201</v>
+      </c>
+      <c r="N4" s="2">
+        <v>303</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2">
+        <v>2</v>
+      </c>
+      <c r="S4" s="30">
+        <v>103</v>
+      </c>
+      <c r="T4" s="2">
+        <v>201</v>
+      </c>
+      <c r="U4" s="2">
+        <v>303</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W4" s="2">
+        <v>1</v>
+      </c>
+      <c r="X4" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="2"/>
+    </row>
+    <row r="5" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2</v>
+      </c>
+      <c r="E5" s="34"/>
+      <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="3">
+        <v>103</v>
+      </c>
+      <c r="H5" s="3">
+        <v>4</v>
+      </c>
+      <c r="I5" s="26">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>3</v>
+      </c>
+      <c r="L5" s="2">
+        <v>104</v>
+      </c>
+      <c r="M5" s="2">
+        <v>201</v>
+      </c>
+      <c r="N5" s="2">
+        <v>304</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2">
+        <v>3</v>
+      </c>
+      <c r="S5" s="30">
+        <v>104</v>
+      </c>
+      <c r="T5" s="2">
+        <v>201</v>
+      </c>
+      <c r="U5" s="2">
+        <v>304</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W5" s="2">
+        <v>1</v>
+      </c>
+      <c r="X5" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB5" s="2"/>
+    </row>
+    <row r="6" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D6" s="9">
+        <v>3</v>
+      </c>
+      <c r="E6" s="34"/>
+      <c r="F6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="3">
+        <v>104</v>
+      </c>
+      <c r="H6" s="3">
+        <v>4</v>
+      </c>
+      <c r="I6" s="26">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>4</v>
+      </c>
+      <c r="L6" s="2">
+        <v>101</v>
+      </c>
+      <c r="M6" s="2">
+        <v>202</v>
+      </c>
+      <c r="N6" s="2">
+        <v>301</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2">
+        <v>4</v>
+      </c>
+      <c r="S6" s="30">
+        <v>101</v>
+      </c>
+      <c r="T6" s="2">
+        <v>202</v>
+      </c>
+      <c r="U6" s="2">
+        <v>301</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W6" s="2">
+        <v>1</v>
+      </c>
+      <c r="X6" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB6" s="2"/>
+    </row>
+    <row r="7" spans="2:28" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D7" s="9">
+        <v>4</v>
+      </c>
+      <c r="E7" s="34"/>
+      <c r="F7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="3">
+        <v>105</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="26">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2">
+        <v>5</v>
+      </c>
+      <c r="L7" s="2">
+        <v>102</v>
+      </c>
+      <c r="M7" s="2">
+        <v>202</v>
+      </c>
+      <c r="N7" s="2">
+        <v>302</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2">
+        <v>5</v>
+      </c>
+      <c r="S7" s="30">
+        <v>102</v>
+      </c>
+      <c r="T7" s="2">
+        <v>202</v>
+      </c>
+      <c r="U7" s="2">
+        <v>302</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W7" s="2">
+        <v>1</v>
+      </c>
+      <c r="X7" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="2"/>
+    </row>
+    <row r="8" spans="2:28" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C8" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D8" s="12">
+        <v>5</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="11">
+        <v>101</v>
+      </c>
+      <c r="H8" s="12">
+        <v>2</v>
+      </c>
+      <c r="I8" s="14">
+        <v>5</v>
+      </c>
+      <c r="K8" s="2">
+        <v>6</v>
+      </c>
+      <c r="L8" s="2">
+        <v>103</v>
+      </c>
+      <c r="M8" s="2">
+        <v>202</v>
+      </c>
+      <c r="N8" s="2">
+        <v>303</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2">
+        <v>6</v>
+      </c>
+      <c r="S8" s="30">
+        <v>103</v>
+      </c>
+      <c r="T8" s="2">
+        <v>202</v>
+      </c>
+      <c r="U8" s="2">
+        <v>303</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W8" s="2">
+        <v>1</v>
+      </c>
+      <c r="X8" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB8" s="2"/>
+    </row>
+    <row r="9" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D9" s="8">
+        <v>6</v>
+      </c>
+      <c r="E9" s="34"/>
+      <c r="F9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="4">
+        <v>102</v>
+      </c>
+      <c r="H9" s="8">
+        <v>2</v>
+      </c>
+      <c r="I9" s="16">
+        <v>5</v>
+      </c>
+      <c r="K9" s="2">
+        <v>7</v>
+      </c>
+      <c r="L9" s="2">
+        <v>104</v>
+      </c>
+      <c r="M9" s="2">
+        <v>202</v>
+      </c>
+      <c r="N9" s="2">
+        <v>304</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2">
+        <v>7</v>
+      </c>
+      <c r="S9" s="30">
+        <v>104</v>
+      </c>
+      <c r="T9" s="2">
+        <v>202</v>
+      </c>
+      <c r="U9" s="2">
+        <v>304</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W9" s="2">
+        <v>1</v>
+      </c>
+      <c r="X9" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB9" s="2"/>
+    </row>
+    <row r="10" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D10" s="9">
+        <v>7</v>
+      </c>
+      <c r="E10" s="34"/>
+      <c r="F10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3">
+        <v>103</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="18">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="25"/>
+    </row>
+    <row r="11" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D11" s="9">
+        <v>8</v>
+      </c>
+      <c r="E11" s="34"/>
+      <c r="F11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="3">
+        <v>104</v>
+      </c>
+      <c r="H11" s="3">
+        <v>6</v>
+      </c>
+      <c r="I11" s="26">
+        <v>3</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+    </row>
+    <row r="12" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D12" s="9">
+        <v>9</v>
+      </c>
+      <c r="E12" s="34"/>
+      <c r="F12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="3">
+        <v>105</v>
+      </c>
+      <c r="H12" s="3">
+        <v>6</v>
+      </c>
+      <c r="I12" s="26">
+        <v>3</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+    </row>
+    <row r="13" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="29"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+    </row>
+    <row r="14" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="29"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+    </row>
+    <row r="15" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+    </row>
+    <row r="16" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="28"/>
+      <c r="C16" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+    </row>
+    <row r="17" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+    </row>
+    <row r="18" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="28"/>
+      <c r="C18" s="29">
+        <v>50</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+    </row>
+    <row r="19" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+    </row>
+    <row r="20" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+    </row>
+    <row r="21" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="K21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="S21" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="T21" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="U21" s="31"/>
+      <c r="W21" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+    </row>
+    <row r="22" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="K22" s="2">
+        <v>101</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N22" s="2">
+        <v>2</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2">
+        <v>0</v>
+      </c>
+      <c r="S22" s="2">
+        <v>1</v>
+      </c>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2">
+        <v>0</v>
+      </c>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+    </row>
+    <row r="23" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="K23" s="2">
+        <v>102</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="N23" s="2">
+        <v>3</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2">
+        <v>1</v>
+      </c>
+      <c r="S23" s="2">
+        <v>1</v>
+      </c>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2">
+        <v>1</v>
+      </c>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+    </row>
+    <row r="24" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="K24" s="2">
+        <v>103</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N24" s="2">
+        <v>3</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2">
+        <v>2</v>
+      </c>
+      <c r="S24" s="2">
+        <v>1</v>
+      </c>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2">
+        <v>2</v>
+      </c>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+    </row>
+    <row r="25" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="K25" s="2">
+        <v>104</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="N25" s="2">
+        <v>2</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2">
+        <v>3</v>
+      </c>
+      <c r="S25" s="2">
+        <v>1</v>
+      </c>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2">
+        <v>3</v>
+      </c>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2"/>
+    </row>
+    <row r="26" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2">
+        <v>4</v>
+      </c>
+      <c r="S26" s="2">
+        <v>1</v>
+      </c>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2">
+        <v>4</v>
+      </c>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
+      <c r="AB26" s="2"/>
+    </row>
+    <row r="27" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="K27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2">
+        <v>5</v>
+      </c>
+      <c r="S27" s="2">
+        <v>1</v>
+      </c>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2">
+        <v>5</v>
+      </c>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+    </row>
+    <row r="28" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="K28" s="2">
+        <v>201</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N28" s="2">
+        <v>1</v>
+      </c>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2">
+        <v>6</v>
+      </c>
+      <c r="S28" s="2">
+        <v>1</v>
+      </c>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="K29" s="2">
+        <v>202</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N29" s="2">
+        <v>1</v>
+      </c>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2">
+        <v>7</v>
+      </c>
+      <c r="S29" s="2">
+        <v>1</v>
+      </c>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2">
+        <v>8</v>
+      </c>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="K31" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2">
+        <v>9</v>
+      </c>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="32" spans="2:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H32" s="2"/>

</xml_diff>